<commit_message>
fixed simulation result 1.1
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umeer\Desktop\University\TrustChain-Simulator\Data Collections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F948386-D542-4F6A-BD26-3C9214AFD082}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB1188-F606-421E-9EC1-DE0F467846B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="120" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="3996" yWindow="1728" windowWidth="17280" windowHeight="9024" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -25,10 +25,10 @@
     <sheet name="Set10" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -477,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +536,11 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -624,7 +629,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -638,8 +643,9 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -743,18 +749,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="12" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="13" builtinId="33"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -852,7 +862,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.13510910000000001</c:v>
+                    <c:v>6.8890759999999995E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.13510910000000001</c:v>
@@ -879,7 +889,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.13510910000000001</c:v>
+                    <c:v>6.8890759999999995E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.13510910000000001</c:v>
@@ -920,7 +930,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9319090000000001</c:v>
+                  <c:v>1.4701979999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9319090000000001</c:v>
@@ -5835,7 +5845,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5873,7 +5883,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -5901,7 +5911,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5939,7 +5949,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -14597,11 +14607,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="O8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14734,7 +14744,7 @@
       <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="56">
         <v>3</v>
       </c>
       <c r="O2" s="33">
@@ -19164,8 +19174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19199,19 +19209,19 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
-        <v>1.580570186129</v>
+        <v>1.5297051661450001</v>
       </c>
       <c r="C2" s="32">
         <v>1.580570186129</v>
@@ -19231,22 +19241,22 @@
       <c r="I2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54" t="s">
+      <c r="K2" s="55"/>
+      <c r="L2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="M2" s="55"/>
+      <c r="N2" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="54"/>
+      <c r="O2" s="55"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
-        <v>2.0180437195629999</v>
+        <v>1.7263440361110001</v>
       </c>
       <c r="C3" s="32">
         <v>2.0180437195629999</v>
@@ -19269,22 +19279,22 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="55">
         <v>1.2</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54">
+      <c r="K3" s="55"/>
+      <c r="L3" s="55">
         <v>3</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54">
+      <c r="M3" s="55"/>
+      <c r="N3" s="55">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="54"/>
+      <c r="O3" s="55"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
-        <v>1.1847525198810001</v>
+        <v>1.848763423699</v>
       </c>
       <c r="C4" s="32">
         <v>1.1847525198810001</v>
@@ -19307,22 +19317,22 @@
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="55">
         <v>1.3</v>
       </c>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54">
+      <c r="K4" s="55"/>
+      <c r="L4" s="55">
         <v>4</v>
       </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54">
+      <c r="M4" s="55"/>
+      <c r="N4" s="55">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="54"/>
+      <c r="O4" s="55"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
-        <v>0.82846883627199996</v>
+        <v>1.263641598302</v>
       </c>
       <c r="C5" s="32">
         <v>0.82846883627199996</v>
@@ -19345,22 +19355,22 @@
       <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="55">
         <v>2.36</v>
       </c>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54">
+      <c r="K5" s="55"/>
+      <c r="L5" s="55">
         <v>6</v>
       </c>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54">
+      <c r="M5" s="55"/>
+      <c r="N5" s="55">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="54"/>
+      <c r="O5" s="55"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
-        <v>2.7179876495770001</v>
+        <v>1.525047846398</v>
       </c>
       <c r="C6" s="32">
         <v>2.7179876495770001</v>
@@ -19383,22 +19393,22 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" s="54">
+      <c r="J6" s="55">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54">
+      <c r="K6" s="55"/>
+      <c r="L6" s="55">
         <v>8</v>
       </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54">
+      <c r="M6" s="55"/>
+      <c r="N6" s="55">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="54"/>
+      <c r="O6" s="55"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
-        <v>1.753576188721</v>
+        <v>1.203207808613</v>
       </c>
       <c r="C7" s="32">
         <v>1.753576188721</v>
@@ -19421,22 +19431,22 @@
       <c r="I7">
         <v>1000</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="55">
         <v>3.55</v>
       </c>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54">
+      <c r="K7" s="55"/>
+      <c r="L7" s="55">
         <v>12</v>
       </c>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54">
+      <c r="M7" s="55"/>
+      <c r="N7" s="55">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="54"/>
+      <c r="O7" s="55"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
-        <v>1.457303628837</v>
+        <v>1.8491733109640001</v>
       </c>
       <c r="C8" s="32">
         <v>1.457303628837</v>
@@ -19456,7 +19466,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" s="32">
-        <v>2.7432749945329999</v>
+        <v>1.2352078257120001</v>
       </c>
       <c r="C9" s="32">
         <v>2.7432749945329999</v>
@@ -19476,7 +19486,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" s="32">
-        <v>1.7998201072469999</v>
+        <v>1.7492208336870001</v>
       </c>
       <c r="C10" s="32">
         <v>1.7998201072469999</v>
@@ -19496,7 +19506,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="32">
-        <v>2.4694143902849999</v>
+        <v>0.93183882744000002</v>
       </c>
       <c r="C11" s="32">
         <v>2.4694143902849999</v>
@@ -19516,7 +19526,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="32">
-        <v>3.2106662988260002</v>
+        <v>1.7363918421390001</v>
       </c>
       <c r="C12" s="32">
         <v>3.2106662988260002</v>
@@ -19536,7 +19546,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="32">
-        <v>1.265645541636</v>
+        <v>0.78330766388299999</v>
       </c>
       <c r="C13" s="32">
         <v>1.265645541636</v>
@@ -19556,7 +19566,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="32">
-        <v>2.936697945318</v>
+        <v>1.9209648898</v>
       </c>
       <c r="C14" s="32">
         <v>2.936697945318</v>
@@ -19576,7 +19586,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="32">
-        <v>1.4435489697049999</v>
+        <v>1.2505701174949999</v>
       </c>
       <c r="C15" s="32">
         <v>1.4435489697049999</v>
@@ -19596,7 +19606,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="32">
-        <v>1.65524223526</v>
+        <v>1.8069447503960001</v>
       </c>
       <c r="C16" s="32">
         <v>1.65524223526</v>
@@ -19616,7 +19626,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="32">
-        <v>1.260282290523</v>
+        <v>1.2231586629860001</v>
       </c>
       <c r="C17" s="32">
         <v>1.260282290523</v>
@@ -19636,7 +19646,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="32">
-        <v>2.1756362908189999</v>
+        <v>0.96727112336099996</v>
       </c>
       <c r="C18" s="32">
         <v>2.1756362908189999</v>
@@ -19656,7 +19666,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="32">
-        <v>1.659014083904</v>
+        <v>1.7803714215749999</v>
       </c>
       <c r="C19" s="32">
         <v>1.659014083904</v>
@@ -19676,7 +19686,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="32">
-        <v>1.666763935803</v>
+        <v>1.267253996465</v>
       </c>
       <c r="C20" s="32">
         <v>1.666763935803</v>
@@ -19696,7 +19706,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="32">
-        <v>2.3735025309819999</v>
+        <v>1.5989062476310001</v>
       </c>
       <c r="C21" s="32">
         <v>2.3735025309819999</v>
@@ -19716,7 +19726,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="32">
-        <v>1.862353761507</v>
+        <v>1.6682997899859999</v>
       </c>
       <c r="C22" s="32">
         <v>1.862353761507</v>
@@ -19736,7 +19746,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="32">
-        <v>3.1658619439029998</v>
+        <v>1.7739574388670001</v>
       </c>
       <c r="C23" s="32">
         <v>3.1658619439029998</v>
@@ -19756,7 +19766,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="32">
-        <v>1.941892739771</v>
+        <v>1.189906411837</v>
       </c>
       <c r="C24" s="32">
         <v>1.941892739771</v>
@@ -19776,7 +19786,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="32">
-        <v>1.486146077261</v>
+        <v>1.60832598965</v>
       </c>
       <c r="C25" s="32">
         <v>1.486146077261</v>
@@ -19796,7 +19806,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="32">
-        <v>0.81361851142700004</v>
+        <v>1.585718533955</v>
       </c>
       <c r="C26" s="32">
         <v>0.81361851142700004</v>
@@ -19816,7 +19826,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="32">
-        <v>0.93397147029500005</v>
+        <v>1.383405570766</v>
       </c>
       <c r="C27" s="32">
         <v>0.93397147029500005</v>
@@ -19836,7 +19846,7 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="32">
-        <v>1.6351710041980001</v>
+        <v>0.98602623067399997</v>
       </c>
       <c r="C28" s="32">
         <v>1.6351710041980001</v>
@@ -19856,7 +19866,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="32">
-        <v>2.3094689319969999</v>
+        <v>1.3230288092039999</v>
       </c>
       <c r="C29" s="32">
         <v>2.3094689319969999</v>
@@ -19876,7 +19886,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="32">
-        <v>1.3265699689799999</v>
+        <v>1.3109761317990001</v>
       </c>
       <c r="C30" s="32">
         <v>1.3265699689799999</v>
@@ -19896,7 +19906,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="32">
-        <v>3.2561996008329999</v>
+        <v>1.551386970474</v>
       </c>
       <c r="C31" s="32">
         <v>3.2561996008329999</v>
@@ -19916,7 +19926,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="32">
-        <v>2.925316406686</v>
+        <v>1.339392561778</v>
       </c>
       <c r="C32" s="32">
         <v>2.925316406686</v>
@@ -19936,7 +19946,7 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="32">
-        <v>2.2061163494499998</v>
+        <v>1.869192395512</v>
       </c>
       <c r="C33" s="32">
         <v>2.2061163494499998</v>
@@ -19956,7 +19966,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="32">
-        <v>1.046187710396</v>
+        <v>1.808273226102</v>
       </c>
       <c r="C34" s="32">
         <v>1.046187710396</v>
@@ -19976,7 +19986,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="32">
-        <v>1.4134988208170001</v>
+        <v>1.5084261852109999</v>
       </c>
       <c r="C35" s="32">
         <v>1.4134988208170001</v>
@@ -19996,7 +20006,7 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="32">
-        <v>3.2652411969239998</v>
+        <v>1.3966294131570001</v>
       </c>
       <c r="C36" s="32">
         <v>3.2652411969239998</v>
@@ -20016,7 +20026,7 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="32">
-        <v>1.4110999532570001</v>
+        <v>1.0862525709299999</v>
       </c>
       <c r="C37" s="32">
         <v>1.4110999532570001</v>
@@ -20036,7 +20046,7 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="32">
-        <v>1.753438959663</v>
+        <v>1.339891590218</v>
       </c>
       <c r="C38" s="32">
         <v>1.753438959663</v>
@@ -20056,7 +20066,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="32">
-        <v>1.460395246744</v>
+        <v>1.6101712025829999</v>
       </c>
       <c r="C39" s="32">
         <v>1.460395246744</v>
@@ -20076,7 +20086,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="32">
-        <v>2.3270775319000001</v>
+        <v>1.9105397259350001</v>
       </c>
       <c r="C40" s="32">
         <v>2.3270775319000001</v>
@@ -20096,7 +20106,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="32">
-        <v>2.280864005412</v>
+        <v>1.7791316506579999</v>
       </c>
       <c r="C41" s="32">
         <v>2.280864005412</v>
@@ -20116,7 +20126,7 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="32">
-        <v>1.6646319885400001</v>
+        <v>1.3436290443409999</v>
       </c>
       <c r="C42" s="32">
         <v>1.6646319885400001</v>
@@ -20136,7 +20146,7 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="32">
-        <v>1.2704508294679999</v>
+        <v>1.27172572956</v>
       </c>
       <c r="C43" s="32">
         <v>1.2704508294679999</v>
@@ -20156,7 +20166,7 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="32">
-        <v>2.3623122152799998</v>
+        <v>1.863529605124</v>
       </c>
       <c r="C44" s="32">
         <v>2.3623122152799998</v>
@@ -20176,7 +20186,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="32">
-        <v>1.146708701923</v>
+        <v>1.4029948615929999</v>
       </c>
       <c r="C45" s="32">
         <v>1.146708701923</v>
@@ -20196,7 +20206,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="32">
-        <v>1.2384567095000001</v>
+        <v>1.0442943130219999</v>
       </c>
       <c r="C46" s="32">
         <v>1.2384567095000001</v>
@@ -20216,7 +20226,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="32">
-        <v>2.4852251450330001</v>
+        <v>0.93525462135199999</v>
       </c>
       <c r="C47" s="32">
         <v>2.4852251450330001</v>
@@ -20236,7 +20246,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="32">
-        <v>3.168347909235</v>
+        <v>1.3490006240879999</v>
       </c>
       <c r="C48" s="32">
         <v>3.168347909235</v>
@@ -20256,7 +20266,7 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="32">
-        <v>1.075675098864</v>
+        <v>1.91469172534</v>
       </c>
       <c r="C49" s="32">
         <v>1.075675098864</v>
@@ -20276,7 +20286,7 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="32">
-        <v>2.025088849311</v>
+        <v>1.977359599773</v>
       </c>
       <c r="C50" s="32">
         <v>2.025088849311</v>
@@ -20296,7 +20306,7 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="32">
-        <v>1.354263039271</v>
+        <v>1.7506292952689999</v>
       </c>
       <c r="C51" s="32">
         <v>1.354263039271</v>
@@ -20316,7 +20326,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="32">
-        <v>1.0673767964150001</v>
+        <v>2.0120573490060001</v>
       </c>
       <c r="C52" s="32">
         <v>1.0673767964150001</v>
@@ -20336,7 +20346,7 @@
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="32">
-        <v>2.3192041645420001</v>
+        <v>1.352907219662</v>
       </c>
       <c r="C53" s="32">
         <v>2.3192041645420001</v>
@@ -20356,7 +20366,7 @@
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="32">
-        <v>1.2399793549510001</v>
+        <v>1.7191290597090001</v>
       </c>
       <c r="C54" s="32">
         <v>1.2399793549510001</v>
@@ -20376,7 +20386,7 @@
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55">
-        <v>2.8749201569639999</v>
+        <v>1.488797915261</v>
       </c>
       <c r="C55">
         <v>2.8749201569639999</v>
@@ -20396,7 +20406,7 @@
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56">
-        <v>2.5169572029789999</v>
+        <v>0.83789411432000005</v>
       </c>
       <c r="C56">
         <v>2.5169572029789999</v>
@@ -20416,7 +20426,7 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57">
-        <v>1.2814723153459999</v>
+        <v>1.3962037458080001</v>
       </c>
       <c r="C57">
         <v>1.2814723153459999</v>
@@ -20436,7 +20446,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58">
-        <v>1.810248396792</v>
+        <v>1.579298363865</v>
       </c>
       <c r="C58">
         <v>1.810248396792</v>
@@ -20456,7 +20466,7 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59">
-        <v>1.251354533095</v>
+        <v>1.690038551609</v>
       </c>
       <c r="C59">
         <v>1.251354533095</v>
@@ -20476,7 +20486,7 @@
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>1.3827071310950001</v>
+        <v>0.96991391764699997</v>
       </c>
       <c r="C60">
         <v>1.3827071310950001</v>
@@ -20496,7 +20506,7 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61">
-        <v>1.4866675524240001</v>
+        <v>1.2345316689329999</v>
       </c>
       <c r="C61">
         <v>1.4866675524240001</v>
@@ -20516,7 +20526,7 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62">
-        <v>2.5607889070500001</v>
+        <v>1.1176951398070001</v>
       </c>
       <c r="C62">
         <v>2.5607889070500001</v>
@@ -20536,7 +20546,7 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63">
-        <v>1.4808248718270001</v>
+        <v>1.0379566818470001</v>
       </c>
       <c r="C63">
         <v>1.4808248718270001</v>
@@ -20556,7 +20566,7 @@
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64">
-        <v>2.2849940438490002</v>
+        <v>0.92625273208600001</v>
       </c>
       <c r="C64">
         <v>2.2849940438490002</v>
@@ -20576,7 +20586,7 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65">
-        <v>1.2275861220769999</v>
+        <v>1.73805986714</v>
       </c>
       <c r="C65">
         <v>1.2275861220769999</v>
@@ -20596,7 +20606,7 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66">
-        <v>1.3367381915450001</v>
+        <v>1.823179395071</v>
       </c>
       <c r="C66">
         <v>1.3367381915450001</v>
@@ -20616,7 +20626,7 @@
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67">
-        <v>3.6529464896429999</v>
+        <v>1.2117767027449999</v>
       </c>
       <c r="C67">
         <v>3.6529464896429999</v>
@@ -20636,7 +20646,7 @@
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68">
-        <v>3.4019565098050002</v>
+        <v>0.64502590127699999</v>
       </c>
       <c r="C68">
         <v>3.4019565098050002</v>
@@ -20656,7 +20666,7 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69">
-        <v>1.474626015306</v>
+        <v>1.327399842161</v>
       </c>
       <c r="C69">
         <v>1.474626015306</v>
@@ -20676,7 +20686,7 @@
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70">
-        <v>1.8755567386880001</v>
+        <v>1.552031536666</v>
       </c>
       <c r="C70">
         <v>1.8755567386880001</v>
@@ -20696,7 +20706,7 @@
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71">
-        <v>2.2167430258019998</v>
+        <v>1.9595237095439999</v>
       </c>
       <c r="C71">
         <v>2.2167430258019998</v>
@@ -20716,7 +20726,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72">
-        <v>1.816344885188</v>
+        <v>1.9539402161320001</v>
       </c>
       <c r="C72">
         <v>1.816344885188</v>
@@ -20736,7 +20746,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73">
-        <v>2.0937557375320002</v>
+        <v>1.9436852153519999</v>
       </c>
       <c r="C73">
         <v>2.0937557375320002</v>
@@ -20756,7 +20766,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74">
-        <v>2.545938764872</v>
+        <v>1.1764924981160001</v>
       </c>
       <c r="C74">
         <v>2.545938764872</v>
@@ -20776,7 +20786,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75">
-        <v>2.1479593014009999</v>
+        <v>1.9545154770569999</v>
       </c>
       <c r="C75">
         <v>2.1479593014009999</v>
@@ -20796,7 +20806,7 @@
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76">
-        <v>2.46298743978</v>
+        <v>1.841078346462</v>
       </c>
       <c r="C76">
         <v>2.46298743978</v>
@@ -20816,7 +20826,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77">
-        <v>1.2594297738410001</v>
+        <v>1.348446148541</v>
       </c>
       <c r="C77">
         <v>1.2594297738410001</v>
@@ -20836,7 +20846,7 @@
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78">
-        <v>1.2263011508620001</v>
+        <v>2.4263653311210001</v>
       </c>
       <c r="C78">
         <v>1.2263011508620001</v>
@@ -20856,7 +20866,7 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79">
-        <v>1.3739606578779999</v>
+        <v>1.180176883104</v>
       </c>
       <c r="C79">
         <v>1.3739606578779999</v>
@@ -20876,7 +20886,7 @@
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80">
-        <v>3.337014082879</v>
+        <v>1.4058633509089999</v>
       </c>
       <c r="C80">
         <v>3.337014082879</v>
@@ -20896,7 +20906,7 @@
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81">
-        <v>0.97219825641799995</v>
+        <v>1.9100637891459999</v>
       </c>
       <c r="C81">
         <v>0.97219825641799995</v>
@@ -20916,7 +20926,7 @@
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82">
-        <v>1.494016681817</v>
+        <v>1.392067893541</v>
       </c>
       <c r="C82">
         <v>1.494016681817</v>
@@ -20936,7 +20946,7 @@
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83">
-        <v>2.6352032306669999</v>
+        <v>1.773619324055</v>
       </c>
       <c r="C83">
         <v>2.6352032306669999</v>
@@ -20956,7 +20966,7 @@
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84">
-        <v>1.2078665124779999</v>
+        <v>1.603455320353</v>
       </c>
       <c r="C84">
         <v>1.2078665124779999</v>
@@ -20976,7 +20986,7 @@
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B85">
-        <v>1.8400117769040001</v>
+        <v>0.81624535888899996</v>
       </c>
       <c r="C85">
         <v>1.8400117769040001</v>
@@ -20996,7 +21006,7 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86">
-        <v>1.354191492172</v>
+        <v>1.159619780916</v>
       </c>
       <c r="C86">
         <v>1.354191492172</v>
@@ -21016,7 +21026,7 @@
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87">
-        <v>1.0278337569439999</v>
+        <v>1.6068763816389999</v>
       </c>
       <c r="C87">
         <v>1.0278337569439999</v>
@@ -21036,7 +21046,7 @@
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B88">
-        <v>2.363315038928</v>
+        <v>1.3993724405829999</v>
       </c>
       <c r="C88">
         <v>2.363315038928</v>
@@ -21056,7 +21066,7 @@
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B89">
-        <v>1.706487349294</v>
+        <v>1.7945763772350001</v>
       </c>
       <c r="C89">
         <v>1.706487349294</v>
@@ -21076,7 +21086,7 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90">
-        <v>2.6914045008760001</v>
+        <v>0.77814805388599995</v>
       </c>
       <c r="C90">
         <v>2.6914045008760001</v>
@@ -21096,7 +21106,7 @@
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91">
-        <v>1.6966235380020001</v>
+        <v>1.906087127178</v>
       </c>
       <c r="C91">
         <v>1.6966235380020001</v>
@@ -21116,7 +21126,7 @@
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B92">
-        <v>3.1492678152920002</v>
+        <v>1.5867168592550001</v>
       </c>
       <c r="C92">
         <v>3.1492678152920002</v>
@@ -21136,7 +21146,7 @@
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B93">
-        <v>2.167947390503</v>
+        <v>1.591443404049</v>
       </c>
       <c r="C93">
         <v>2.167947390503</v>
@@ -21156,7 +21166,7 @@
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B94">
-        <v>2.1333477081529999</v>
+        <v>1.618629995094</v>
       </c>
       <c r="C94">
         <v>2.1333477081529999</v>
@@ -21176,7 +21186,7 @@
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B95">
-        <v>2.3462676266939999</v>
+        <v>1.2186089881560001</v>
       </c>
       <c r="C95">
         <v>2.3462676266939999</v>
@@ -21196,7 +21206,7 @@
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B96">
-        <v>1.3540386912939999</v>
+        <v>1.3046223043459999</v>
       </c>
       <c r="C96">
         <v>1.3540386912939999</v>
@@ -21216,7 +21226,7 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B97">
-        <v>1.467974982908</v>
+        <v>1.8290622486200001</v>
       </c>
       <c r="C97">
         <v>1.467974982908</v>
@@ -21236,7 +21246,7 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B98">
-        <v>3.1116442665399999</v>
+        <v>0.87523857032399999</v>
       </c>
       <c r="C98">
         <v>3.1116442665399999</v>
@@ -21256,7 +21266,7 @@
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99">
-        <v>2.1924741243270001</v>
+        <v>0.98972674342099998</v>
       </c>
       <c r="C99">
         <v>2.1924741243270001</v>
@@ -21276,7 +21286,7 @@
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B100">
-        <v>1.8794539722950001</v>
+        <v>1.6128448780689999</v>
       </c>
       <c r="C100">
         <v>1.8794539722950001</v>
@@ -21296,7 +21306,7 @@
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101">
-        <v>2.5801294244880002</v>
+        <v>1.323200887714</v>
       </c>
       <c r="C101">
         <v>2.5801294244880002</v>
@@ -21316,7 +21326,7 @@
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103">
-        <v>1.9319090000000001</v>
+        <v>1.4701979999999999</v>
       </c>
       <c r="C103">
         <v>1.9319090000000001</v>
@@ -21336,7 +21346,7 @@
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B104">
-        <v>0.68934479999999998</v>
+        <v>0.35148990000000002</v>
       </c>
       <c r="C104">
         <v>0.68934479999999998</v>
@@ -21356,7 +21366,7 @@
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105">
-        <v>0.13510910000000001</v>
+        <v>6.8890759999999995E-2</v>
       </c>
       <c r="C105">
         <v>0.13510910000000001</v>
@@ -21376,7 +21386,7 @@
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B106">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C106">
         <v>85</v>
@@ -21396,7 +21406,7 @@
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C107">
         <v>15</v>
@@ -21416,6 +21426,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -21426,15 +21445,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21445,7 +21455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8ADDF3-F6DC-49DE-90F6-6F07047D1F12}">
   <dimension ref="A1:J2007"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
@@ -21487,12 +21497,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
@@ -36693,7 +36703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB14316-39CC-412C-A762-31F37CE381A2}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
@@ -51214,7 +51224,7 @@
   <dimension ref="A1:AA218"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
inserted evaluaiton detail for set 11
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB1188-F606-421E-9EC1-DE0F467846B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB17531-AA3A-4179-ACA5-E284637CE27C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3996" yWindow="1728" windowWidth="17280" windowHeight="9024" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -25,10 +25,10 @@
     <sheet name="Set10" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="105">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>1000000kbps</t>
-  </si>
-  <si>
-    <t>Detection Time [AVG]</t>
   </si>
   <si>
     <t>Set</t>
@@ -172,9 +169,6 @@
     <t>SET4.1</t>
   </si>
   <si>
-    <t>Extra</t>
-  </si>
-  <si>
     <t>5 - Test execution time</t>
   </si>
   <si>
@@ -233,12 +227,6 @@
   </si>
   <si>
     <t>Count</t>
-  </si>
-  <si>
-    <t>Exection time: 2.5 Min</t>
-  </si>
-  <si>
-    <t>Exection time: 14 s</t>
   </si>
   <si>
     <t>Data Ordered</t>
@@ -317,25 +305,10 @@
     <t>9 -  Average Path Length</t>
   </si>
   <si>
-    <t>anonymusAuditingTimeoutTime</t>
-  </si>
-  <si>
-    <t>transactionTimeoutTime</t>
-  </si>
-  <si>
-    <t>anonymizerDisseminationTime</t>
-  </si>
-  <si>
-    <t>anonymizerLifeTime</t>
-  </si>
-  <si>
     <t>uniform(60s, 120s)</t>
   </si>
   <si>
     <t>120s</t>
-  </si>
-  <si>
-    <t>numberOfAnonymizer</t>
   </si>
   <si>
     <t>10 - Variation of Anonymizer nodes</t>
@@ -360,6 +333,42 @@
   </si>
   <si>
     <t>Results:</t>
+  </si>
+  <si>
+    <t>11 - Evil Anonimizer</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>1000s</t>
+  </si>
+  <si>
+    <t>Number Of Anonymizer</t>
+  </si>
+  <si>
+    <t>Anonymus Auditing Timeout Time</t>
+  </si>
+  <si>
+    <t>Transaction Timeout Time</t>
+  </si>
+  <si>
+    <t>Anonimizer Number Threshold</t>
+  </si>
+  <si>
+    <t>Probability Evil Anonimizer</t>
+  </si>
+  <si>
+    <t>Sim Time</t>
+  </si>
+  <si>
+    <t>Anonymizer Life Time</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Anonymizer Dissemination Time</t>
   </si>
 </sst>
 </file>
@@ -540,7 +549,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -643,9 +653,9 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +725,9 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,22 +762,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
+    <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="12" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="13" builtinId="33"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -5845,7 +5866,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5883,7 +5904,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -5911,7 +5932,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5949,7 +5970,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -14605,13 +14626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T30" sqref="T30"/>
+      <selection pane="bottomRight" activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14629,19 +14650,20 @@
     <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.5546875" customWidth="1"/>
     <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="28" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -14659,7 +14681,7 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>0</v>
@@ -14680,33 +14702,36 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>39</v>
+        <v>100</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>19</v>
+      <c r="A2" s="48" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -14744,7 +14769,7 @@
       <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="56">
+      <c r="N2">
         <v>3</v>
       </c>
       <c r="O2" s="33">
@@ -14754,17 +14779,27 @@
         <v>60</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S2" s="1">
         <v>100</v>
       </c>
+      <c r="T2">
+        <f>N2</f>
+        <v>3</v>
+      </c>
+      <c r="U2" s="58">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14811,17 +14846,27 @@
         <v>60</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S3" s="28">
         <v>100</v>
       </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T60" si="1">N3</f>
+        <v>10</v>
+      </c>
+      <c r="U3" s="58">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14829,7 +14874,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D37" si="1">2*LOG(C4)/(C4-1)</f>
+        <f t="shared" ref="D4:D37" si="2">2*LOG(C4)/(C4-1)</f>
         <v>6.9345714462694649E-2</v>
       </c>
       <c r="E4" s="1">
@@ -14868,19 +14913,28 @@
         <v>60</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S4" s="28">
         <v>100</v>
       </c>
-      <c r="V4" s="1"/>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U4" s="58">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>94</v>
+      </c>
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -14888,7 +14942,7 @@
         <v>100</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0404040404040407E-2</v>
       </c>
       <c r="E5" s="1">
@@ -14927,18 +14981,28 @@
         <v>60</v>
       </c>
       <c r="Q5" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R5" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S5" s="28">
         <v>100</v>
       </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U5" s="58">
+        <v>0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>94</v>
+      </c>
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -14946,11 +15010,11 @@
         <v>500</v>
       </c>
       <c r="D6" s="28">
-        <f t="shared" ref="D6" si="2">2*LOG(C6)/(C6-1)</f>
+        <f t="shared" ref="D6" si="3">2*LOG(C6)/(C6-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E6" s="28">
-        <f t="shared" ref="E6" si="3">LN(C6)/(C6)</f>
+        <f t="shared" ref="E6" si="4">LN(C6)/(C6)</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F6" s="28">
@@ -14986,18 +15050,28 @@
         <v>60</v>
       </c>
       <c r="Q6" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R6" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S6" s="28">
         <v>100</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U6" s="58">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>94</v>
+      </c>
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15005,7 +15079,7 @@
         <v>1000</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.006006006006006E-3</v>
       </c>
       <c r="E7" s="1">
@@ -15045,18 +15119,28 @@
         <v>60</v>
       </c>
       <c r="Q7" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R7" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S7" s="28">
         <v>100</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U7" s="58">
+        <v>0</v>
+      </c>
+      <c r="V7" t="s">
+        <v>94</v>
+      </c>
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -15064,7 +15148,7 @@
         <v>10000</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0008000800080011E-4</v>
       </c>
       <c r="E8" s="1">
@@ -15101,19 +15185,29 @@
         <v>60</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R8" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S8" s="28">
         <v>100</v>
       </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U8" s="58">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>94</v>
+      </c>
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="53" t="s">
-        <v>20</v>
+      <c r="A9" s="54" t="s">
+        <v>19</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -15162,18 +15256,28 @@
         <v>60</v>
       </c>
       <c r="Q9" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R9" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S9" s="28">
         <v>100</v>
       </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U9" s="58">
+        <v>0</v>
+      </c>
+      <c r="V9" t="s">
+        <v>94</v>
+      </c>
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -15189,7 +15293,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F10" s="28">
-        <f t="shared" ref="F10:F48" si="4">E10</f>
+        <f t="shared" ref="F10:F48" si="5">E10</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G10" s="18"/>
@@ -15221,18 +15325,28 @@
         <v>60</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R10" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S10" s="28">
         <v>100</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U10" s="58">
+        <v>0</v>
+      </c>
+      <c r="V10" t="s">
+        <v>94</v>
+      </c>
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -15240,7 +15354,7 @@
         <v>500</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E11" s="1">
@@ -15248,7 +15362,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F11" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G11" s="18"/>
@@ -15280,18 +15394,28 @@
         <v>60</v>
       </c>
       <c r="Q11" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R11" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S11" s="28">
         <v>100</v>
       </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U11" s="58">
+        <v>0</v>
+      </c>
+      <c r="V11" t="s">
+        <v>94</v>
+      </c>
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -15299,7 +15423,7 @@
         <v>500</v>
       </c>
       <c r="D12" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E12" s="22">
@@ -15307,7 +15431,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F12" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G12" s="22"/>
@@ -15339,19 +15463,29 @@
         <v>60</v>
       </c>
       <c r="Q12" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R12" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S12" s="28">
         <v>100</v>
       </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U12" s="58">
+        <v>0</v>
+      </c>
+      <c r="V12" t="s">
+        <v>94</v>
+      </c>
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
-        <v>21</v>
+      <c r="A13" s="50" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -15360,7 +15494,7 @@
         <v>500</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E13" s="1">
@@ -15368,7 +15502,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F13" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G13" s="18"/>
@@ -15400,17 +15534,27 @@
         <v>60</v>
       </c>
       <c r="Q13" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R13" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S13" s="28">
         <v>100</v>
       </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U13" s="58">
+        <v>0</v>
+      </c>
+      <c r="V13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -15418,7 +15562,7 @@
         <v>500</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E14" s="1">
@@ -15426,7 +15570,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F14" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G14" s="18"/>
@@ -15443,7 +15587,7 @@
         <v>8</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>10</v>
@@ -15458,17 +15602,27 @@
         <v>60</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R14" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S14" s="28">
         <v>100</v>
       </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U14" s="58">
+        <v>0</v>
+      </c>
+      <c r="V14" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -15476,7 +15630,7 @@
         <v>500</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E15" s="1">
@@ -15484,7 +15638,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F15" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G15" s="18"/>
@@ -15501,7 +15655,7 @@
         <v>8</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>10</v>
@@ -15516,17 +15670,27 @@
         <v>60</v>
       </c>
       <c r="Q15" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R15" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S15" s="28">
         <v>100</v>
       </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U15" s="58">
+        <v>0</v>
+      </c>
+      <c r="V15" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -15534,7 +15698,7 @@
         <v>500</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E16" s="1">
@@ -15542,7 +15706,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F16" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G16" s="18"/>
@@ -15559,7 +15723,7 @@
         <v>8</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>10</v>
@@ -15574,17 +15738,27 @@
         <v>60</v>
       </c>
       <c r="Q16" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R16" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S16" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U16" s="58">
+        <v>0</v>
+      </c>
+      <c r="V16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="50"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -15592,7 +15766,7 @@
         <v>500</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E17" s="1">
@@ -15600,7 +15774,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F17" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G17" s="18"/>
@@ -15632,17 +15806,27 @@
         <v>60</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R17" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S17" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U17" s="58">
+        <v>0</v>
+      </c>
+      <c r="V17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -15650,7 +15834,7 @@
         <v>500</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E18" s="1">
@@ -15658,7 +15842,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F18" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G18" s="18"/>
@@ -15690,18 +15874,28 @@
         <v>60</v>
       </c>
       <c r="Q18" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R18" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S18" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U18" s="58">
+        <v>0</v>
+      </c>
+      <c r="V18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
@@ -15710,7 +15904,7 @@
         <v>500</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E19" s="1">
@@ -15718,7 +15912,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F19" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G19" s="18"/>
@@ -15750,18 +15944,28 @@
         <v>60</v>
       </c>
       <c r="Q19" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R19" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S19" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52" t="s">
-        <v>40</v>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U19" s="58">
+        <v>0</v>
+      </c>
+      <c r="V19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="53" t="s">
+        <v>38</v>
       </c>
       <c r="B20" s="16">
         <v>1</v>
@@ -15770,7 +15974,7 @@
         <v>500</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E20" s="1">
@@ -15778,7 +15982,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F20" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G20" s="18"/>
@@ -15810,20 +16014,27 @@
         <v>60</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R20" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S20" s="28">
         <v>100</v>
       </c>
-      <c r="U20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U20" s="58">
+        <v>0</v>
+      </c>
+      <c r="V20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
       <c r="B21" s="16">
         <v>2</v>
       </c>
@@ -15831,7 +16042,7 @@
         <v>500</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E21" s="1">
@@ -15839,7 +16050,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F21" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G21" s="18"/>
@@ -15871,21 +16082,28 @@
         <v>60</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R21" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S21" s="28">
         <v>100</v>
       </c>
-      <c r="U21" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
-        <v>41</v>
+      <c r="T21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U21" s="58">
+        <v>0</v>
+      </c>
+      <c r="V21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="51" t="s">
+        <v>39</v>
       </c>
       <c r="B22" s="10">
         <v>1</v>
@@ -15894,7 +16112,7 @@
         <v>500</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E22" s="1">
@@ -15902,7 +16120,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F22" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G22" s="18"/>
@@ -15916,7 +16134,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>7</v>
@@ -15934,17 +16152,27 @@
         <v>60</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R22" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S22" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+      <c r="T22">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U22" s="58">
+        <v>0</v>
+      </c>
+      <c r="V22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="51"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -15952,7 +16180,7 @@
         <v>500</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E23" s="1">
@@ -15960,7 +16188,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F23" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G23" s="18"/>
@@ -15974,7 +16202,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>7</v>
@@ -15992,17 +16220,27 @@
         <v>60</v>
       </c>
       <c r="Q23" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R23" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S23" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U23" s="58">
+        <v>0</v>
+      </c>
+      <c r="V23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -16010,7 +16248,7 @@
         <v>500</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E24" s="1">
@@ -16018,7 +16256,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F24" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G24" s="18"/>
@@ -16050,17 +16288,27 @@
         <v>60</v>
       </c>
       <c r="Q24" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R24" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S24" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U24" s="58">
+        <v>0</v>
+      </c>
+      <c r="V24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -16068,7 +16316,7 @@
         <v>500</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E25" s="1">
@@ -16076,7 +16324,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F25" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G25" s="18"/>
@@ -16090,7 +16338,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>7</v>
@@ -16108,17 +16356,27 @@
         <v>60</v>
       </c>
       <c r="Q25" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R25" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S25" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U25" s="58">
+        <v>0</v>
+      </c>
+      <c r="V25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -16126,7 +16384,7 @@
         <v>500</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E26" s="1">
@@ -16134,7 +16392,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G26" s="18"/>
@@ -16148,7 +16406,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>7</v>
@@ -16166,18 +16424,28 @@
         <v>600</v>
       </c>
       <c r="Q26" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R26" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S26" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" s="51" t="s">
-        <v>50</v>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U26" s="58">
+        <v>0</v>
+      </c>
+      <c r="V26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="52" t="s">
+        <v>48</v>
       </c>
       <c r="B27" s="12">
         <v>1</v>
@@ -16194,7 +16462,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F27" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G27" s="18"/>
@@ -16226,18 +16494,27 @@
         <v>60</v>
       </c>
       <c r="Q27" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R27" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S27" s="28">
         <v>100</v>
       </c>
-      <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U27" s="58">
+        <v>0</v>
+      </c>
+      <c r="V27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A28" s="52"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -16253,7 +16530,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F28" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G28" s="18"/>
@@ -16285,17 +16562,27 @@
         <v>60</v>
       </c>
       <c r="Q28" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R28" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S28" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U28" s="58">
+        <v>0</v>
+      </c>
+      <c r="V28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -16303,7 +16590,7 @@
         <v>500</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E29" s="1">
@@ -16311,7 +16598,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F29" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G29" s="18"/>
@@ -16343,17 +16630,27 @@
         <v>60</v>
       </c>
       <c r="Q29" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R29" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S29" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U29" s="58">
+        <v>0</v>
+      </c>
+      <c r="V29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="52"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -16361,7 +16658,7 @@
         <v>500</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E30" s="1">
@@ -16369,7 +16666,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F30" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G30" s="18"/>
@@ -16401,17 +16698,27 @@
         <v>60</v>
       </c>
       <c r="Q30" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S30" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U30" s="58">
+        <v>0</v>
+      </c>
+      <c r="V30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="52"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -16419,7 +16726,7 @@
         <v>500</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E31" s="1">
@@ -16427,7 +16734,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F31" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G31" s="18"/>
@@ -16459,17 +16766,27 @@
         <v>60</v>
       </c>
       <c r="Q31" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R31" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S31" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U31" s="58">
+        <v>0</v>
+      </c>
+      <c r="V31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -16477,7 +16794,7 @@
         <v>500</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E32" s="1">
@@ -16485,7 +16802,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F32" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G32" s="18"/>
@@ -16517,18 +16834,28 @@
         <v>60</v>
       </c>
       <c r="Q32" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R32" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S32" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="s">
-        <v>51</v>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U32" s="58">
+        <v>0</v>
+      </c>
+      <c r="V32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A33" s="47" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="14">
         <v>1</v>
@@ -16537,7 +16864,7 @@
         <v>500</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E33" s="1">
@@ -16545,7 +16872,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F33" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G33" s="18"/>
@@ -16565,7 +16892,7 @@
         <v>7</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N33" s="33">
         <v>10</v>
@@ -16577,17 +16904,27 @@
         <v>60</v>
       </c>
       <c r="Q33" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R33" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S33" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U33" s="58">
+        <v>0</v>
+      </c>
+      <c r="V33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A34" s="47"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -16595,7 +16932,7 @@
         <v>500</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E34" s="1">
@@ -16603,7 +16940,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F34" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G34" s="18"/>
@@ -16623,7 +16960,7 @@
         <v>7</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N34" s="33">
         <v>10</v>
@@ -16635,17 +16972,27 @@
         <v>60</v>
       </c>
       <c r="Q34" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R34" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S34" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
+      <c r="T34">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U34" s="58">
+        <v>0</v>
+      </c>
+      <c r="V34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A35" s="47"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -16653,7 +17000,7 @@
         <v>500</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E35" s="1">
@@ -16661,7 +17008,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F35" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G35" s="18"/>
@@ -16681,7 +17028,7 @@
         <v>7</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N35" s="33">
         <v>10</v>
@@ -16693,17 +17040,27 @@
         <v>60</v>
       </c>
       <c r="Q35" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S35" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="46"/>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U35" s="58">
+        <v>0</v>
+      </c>
+      <c r="V35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A36" s="47"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -16711,7 +17068,7 @@
         <v>500</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E36" s="1">
@@ -16719,7 +17076,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F36" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G36" s="18"/>
@@ -16739,7 +17096,7 @@
         <v>7</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N36" s="33">
         <v>10</v>
@@ -16751,17 +17108,27 @@
         <v>60</v>
       </c>
       <c r="Q36" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S36" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
+      <c r="T36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U36" s="58">
+        <v>0</v>
+      </c>
+      <c r="V36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A37" s="47"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -16769,7 +17136,7 @@
         <v>500</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E37" s="1">
@@ -16777,7 +17144,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F37" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G37" s="18"/>
@@ -16797,7 +17164,7 @@
         <v>7</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N37" s="33">
         <v>10</v>
@@ -16809,18 +17176,28 @@
         <v>60</v>
       </c>
       <c r="Q37" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R37" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S37" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38" s="45" t="s">
-        <v>84</v>
+      <c r="T37">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U37" s="58">
+        <v>0</v>
+      </c>
+      <c r="V37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A38" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="B38" s="19">
         <v>1</v>
@@ -16834,7 +17211,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F38" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G38" s="18">
@@ -16868,17 +17245,27 @@
         <v>60</v>
       </c>
       <c r="Q38" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R38" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S38" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="T38">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U38" s="58">
+        <v>0</v>
+      </c>
+      <c r="V38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A39" s="46"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -16891,7 +17278,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F39" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G39" s="18">
@@ -16925,17 +17312,27 @@
         <v>60</v>
       </c>
       <c r="Q39" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R39" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S39" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+      <c r="T39">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U39" s="58">
+        <v>0</v>
+      </c>
+      <c r="V39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A40" s="46"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -16948,7 +17345,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F40" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G40" s="18">
@@ -16982,17 +17379,27 @@
         <v>60</v>
       </c>
       <c r="Q40" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R40" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S40" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="45"/>
+      <c r="T40">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U40" s="58">
+        <v>0</v>
+      </c>
+      <c r="V40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A41" s="46"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -17005,7 +17412,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F41" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G41" s="18">
@@ -17039,17 +17446,27 @@
         <v>60</v>
       </c>
       <c r="Q41" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R41" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S41" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="T41">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U41" s="58">
+        <v>0</v>
+      </c>
+      <c r="V41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A42" s="46"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -17058,11 +17475,11 @@
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18">
-        <f t="shared" ref="E42:E48" si="5">LN(C42)/(C42)</f>
+        <f t="shared" ref="E42:E48" si="6">LN(C42)/(C42)</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F42" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G42" s="18">
@@ -17096,18 +17513,28 @@
         <v>60</v>
       </c>
       <c r="Q42" s="33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R42" s="33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S42" s="28">
         <v>100</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="44" t="s">
-        <v>85</v>
+      <c r="T42">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U42" s="58">
+        <v>0</v>
+      </c>
+      <c r="V42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="45" t="s">
+        <v>81</v>
       </c>
       <c r="B43" s="23">
         <v>1</v>
@@ -17120,11 +17547,11 @@
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E43" s="20">
+        <f t="shared" si="6"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F43" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F43" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G43" s="20"/>
@@ -17156,17 +17583,27 @@
         <v>60</v>
       </c>
       <c r="Q43" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R43" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S43" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="44"/>
+      <c r="T43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U43" s="58">
+        <v>0</v>
+      </c>
+      <c r="V43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="45"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -17178,11 +17615,11 @@
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E44" s="20">
+        <f t="shared" si="6"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F44" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F44" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G44" s="20"/>
@@ -17214,17 +17651,27 @@
         <v>60</v>
       </c>
       <c r="Q44" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R44" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S44" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="44"/>
+      <c r="T44">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U44" s="58">
+        <v>0</v>
+      </c>
+      <c r="V44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="45"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -17232,15 +17679,15 @@
         <v>500</v>
       </c>
       <c r="D45" s="20">
-        <f t="shared" ref="D45:D47" si="6">2*LOG(C45)/(C45-1)</f>
+        <f t="shared" ref="D45:D47" si="7">2*LOG(C45)/(C45-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E45" s="20">
+        <f t="shared" si="6"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F45" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F45" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G45" s="20"/>
@@ -17272,17 +17719,27 @@
         <v>60</v>
       </c>
       <c r="Q45" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R45" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S45" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="44"/>
+      <c r="T45">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U45" s="58">
+        <v>0</v>
+      </c>
+      <c r="V45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="45"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -17290,15 +17747,15 @@
         <v>500</v>
       </c>
       <c r="D46" s="20">
+        <f t="shared" si="7"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E46" s="20">
         <f t="shared" si="6"/>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E46" s="20">
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F46" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F46" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G46" s="20"/>
@@ -17330,17 +17787,27 @@
         <v>60</v>
       </c>
       <c r="Q46" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R46" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S46" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="44"/>
+      <c r="T46">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U46" s="58">
+        <v>0</v>
+      </c>
+      <c r="V46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="45"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -17348,15 +17815,15 @@
         <v>500</v>
       </c>
       <c r="D47" s="22">
+        <f t="shared" si="7"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E47" s="22">
         <f t="shared" si="6"/>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E47" s="22">
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F47" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F47" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G47" s="22"/>
@@ -17388,17 +17855,27 @@
         <v>60</v>
       </c>
       <c r="Q47" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R47" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S47" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="44"/>
+      <c r="T47">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U47" s="58">
+        <v>0</v>
+      </c>
+      <c r="V47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="45"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -17407,11 +17884,11 @@
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22">
+        <f t="shared" si="6"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F48" s="28">
         <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F48" s="28">
-        <f t="shared" si="4"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G48" s="22"/>
@@ -17443,18 +17920,28 @@
         <v>60</v>
       </c>
       <c r="Q48" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R48" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S48" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
+      <c r="T48">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U48" s="58">
+        <v>0</v>
+      </c>
+      <c r="V48" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A49" s="44" t="s">
+        <v>85</v>
       </c>
       <c r="B49" s="23">
         <v>1</v>
@@ -17494,17 +17981,27 @@
         <v>60</v>
       </c>
       <c r="Q49" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R49" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S49" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="43"/>
+      <c r="T49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U49" s="58">
+        <v>0</v>
+      </c>
+      <c r="V49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A50" s="44"/>
       <c r="B50" s="23">
         <v>2</v>
       </c>
@@ -17539,17 +18036,27 @@
         <v>60</v>
       </c>
       <c r="Q50" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R50" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S50" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="43"/>
+      <c r="T50">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U50" s="58">
+        <v>0</v>
+      </c>
+      <c r="V50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A51" s="44"/>
       <c r="B51" s="23">
         <v>3</v>
       </c>
@@ -17584,17 +18091,27 @@
         <v>60</v>
       </c>
       <c r="Q51" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R51" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S51" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="43"/>
+      <c r="T51">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="U51" s="58">
+        <v>0</v>
+      </c>
+      <c r="V51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A52" s="44"/>
       <c r="B52" s="23">
         <v>4</v>
       </c>
@@ -17620,7 +18137,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="37" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="O52" s="37">
         <v>30</v>
@@ -17629,25 +18146,688 @@
         <v>60</v>
       </c>
       <c r="Q52" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R52" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S52" s="37">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H53" s="37"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
+      <c r="T52" s="61" t="str">
+        <f t="shared" si="1"/>
+        <v>Max</v>
+      </c>
+      <c r="U52" s="58">
+        <v>0</v>
+      </c>
+      <c r="V52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A53" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="59">
+        <v>1</v>
+      </c>
+      <c r="C53" s="43">
+        <v>500</v>
+      </c>
+      <c r="H53" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I53" s="43">
+        <v>100</v>
+      </c>
+      <c r="J53" s="43">
+        <v>0</v>
+      </c>
+      <c r="K53" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L53" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N53" s="43">
+        <v>30</v>
+      </c>
+      <c r="O53" s="43">
+        <v>30</v>
+      </c>
+      <c r="P53" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q53" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R53" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S53" s="43">
+        <v>100</v>
+      </c>
+      <c r="T53">
+        <f>N53*0.3</f>
+        <v>9</v>
+      </c>
+      <c r="U53" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="V53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A54" s="57"/>
+      <c r="B54" s="59">
+        <v>2</v>
+      </c>
+      <c r="C54" s="43">
+        <v>500</v>
+      </c>
+      <c r="H54" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I54" s="43">
+        <v>100</v>
+      </c>
+      <c r="J54" s="43">
+        <v>0</v>
+      </c>
+      <c r="K54" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L54" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N54" s="43">
+        <v>30</v>
+      </c>
+      <c r="O54" s="43">
+        <v>30</v>
+      </c>
+      <c r="P54" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q54" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R54" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S54" s="43">
+        <v>100</v>
+      </c>
+      <c r="T54">
+        <f>N54*0.5</f>
+        <v>15</v>
+      </c>
+      <c r="U54" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="V54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A55" s="57"/>
+      <c r="B55" s="59">
+        <v>3</v>
+      </c>
+      <c r="C55" s="43">
+        <v>500</v>
+      </c>
+      <c r="H55" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I55" s="43">
+        <v>100</v>
+      </c>
+      <c r="J55" s="43">
+        <v>0</v>
+      </c>
+      <c r="K55" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L55" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N55" s="43">
+        <v>30</v>
+      </c>
+      <c r="O55" s="43">
+        <v>30</v>
+      </c>
+      <c r="P55" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q55" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R55" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S55" s="43">
+        <v>100</v>
+      </c>
+      <c r="T55">
+        <f>N55*0.8</f>
+        <v>24</v>
+      </c>
+      <c r="U55" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="V55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A56" s="57"/>
+      <c r="B56" s="59">
+        <v>4</v>
+      </c>
+      <c r="C56" s="43">
+        <v>500</v>
+      </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
+      <c r="H56" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I56" s="43">
+        <v>100</v>
+      </c>
+      <c r="J56" s="43">
+        <v>0</v>
+      </c>
+      <c r="K56" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N56" s="43">
+        <v>30</v>
+      </c>
+      <c r="O56" s="43">
+        <v>30</v>
+      </c>
+      <c r="P56" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q56" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R56" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S56" s="43">
+        <v>100</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U56" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="V56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A57" s="57"/>
+      <c r="B57" s="59">
+        <v>5</v>
+      </c>
+      <c r="C57" s="43">
+        <v>500</v>
+      </c>
+      <c r="H57" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" s="43">
+        <v>100</v>
+      </c>
+      <c r="J57" s="43">
+        <v>0</v>
+      </c>
+      <c r="K57" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L57" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" s="43">
+        <v>30</v>
+      </c>
+      <c r="O57" s="43">
+        <v>30</v>
+      </c>
+      <c r="P57" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q57" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R57" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S57" s="43">
+        <v>100</v>
+      </c>
+      <c r="T57">
+        <f>N57*0.3</f>
+        <v>9</v>
+      </c>
+      <c r="U57" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="V57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A58" s="57"/>
+      <c r="B58" s="59">
+        <v>6</v>
+      </c>
+      <c r="C58" s="43">
+        <v>500</v>
+      </c>
+      <c r="H58" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I58" s="43">
+        <v>100</v>
+      </c>
+      <c r="J58" s="43">
+        <v>0</v>
+      </c>
+      <c r="K58" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L58" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M58" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" s="43">
+        <v>30</v>
+      </c>
+      <c r="O58" s="43">
+        <v>30</v>
+      </c>
+      <c r="P58" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q58" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R58" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S58" s="43">
+        <v>100</v>
+      </c>
+      <c r="T58">
+        <f>N58*0.5</f>
+        <v>15</v>
+      </c>
+      <c r="U58" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="V58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A59" s="57"/>
+      <c r="B59" s="59">
+        <v>7</v>
+      </c>
+      <c r="C59" s="43">
+        <v>500</v>
+      </c>
+      <c r="H59" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I59" s="43">
+        <v>100</v>
+      </c>
+      <c r="J59" s="43">
+        <v>0</v>
+      </c>
+      <c r="K59" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L59" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M59" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N59" s="43">
+        <v>30</v>
+      </c>
+      <c r="O59" s="43">
+        <v>30</v>
+      </c>
+      <c r="P59" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q59" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R59" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S59" s="43">
+        <v>100</v>
+      </c>
+      <c r="T59">
+        <f>N59*0.8</f>
+        <v>24</v>
+      </c>
+      <c r="U59" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="V59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A60" s="57"/>
+      <c r="B60" s="59">
+        <v>8</v>
+      </c>
+      <c r="C60" s="43">
+        <v>500</v>
+      </c>
+      <c r="H60" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I60" s="43">
+        <v>100</v>
+      </c>
+      <c r="J60" s="43">
+        <v>0</v>
+      </c>
+      <c r="K60" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L60" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M60" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N60" s="43">
+        <v>30</v>
+      </c>
+      <c r="O60" s="43">
+        <v>30</v>
+      </c>
+      <c r="P60" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q60" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R60" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S60" s="43">
+        <v>100</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U60" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="V60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A61" s="57"/>
+      <c r="B61" s="59">
+        <v>9</v>
+      </c>
+      <c r="C61" s="43">
+        <v>500</v>
+      </c>
+      <c r="H61" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I61" s="43">
+        <v>100</v>
+      </c>
+      <c r="J61" s="43">
+        <v>0</v>
+      </c>
+      <c r="K61" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L61" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M61" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N61" s="43">
+        <v>30</v>
+      </c>
+      <c r="O61" s="43">
+        <v>30</v>
+      </c>
+      <c r="P61" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q61" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R61" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S61" s="43">
+        <v>100</v>
+      </c>
+      <c r="T61">
+        <v>9</v>
+      </c>
+      <c r="U61" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="V61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A62" s="57"/>
+      <c r="B62" s="59">
+        <v>10</v>
+      </c>
+      <c r="C62" s="43">
+        <v>500</v>
+      </c>
+      <c r="H62" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I62" s="43">
+        <v>100</v>
+      </c>
+      <c r="J62" s="43">
+        <v>0</v>
+      </c>
+      <c r="K62" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L62" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M62" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N62" s="43">
+        <v>30</v>
+      </c>
+      <c r="O62" s="43">
+        <v>30</v>
+      </c>
+      <c r="P62" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q62" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R62" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S62" s="43">
+        <v>100</v>
+      </c>
+      <c r="T62">
+        <v>15</v>
+      </c>
+      <c r="U62" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="V62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A63" s="57"/>
+      <c r="B63" s="59">
+        <v>11</v>
+      </c>
+      <c r="C63" s="43">
+        <v>500</v>
+      </c>
+      <c r="H63" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I63" s="43">
+        <v>100</v>
+      </c>
+      <c r="J63" s="43">
+        <v>0</v>
+      </c>
+      <c r="K63" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L63" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M63" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N63" s="43">
+        <v>30</v>
+      </c>
+      <c r="O63" s="43">
+        <v>30</v>
+      </c>
+      <c r="P63" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q63" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R63" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S63" s="43">
+        <v>100</v>
+      </c>
+      <c r="T63">
+        <v>24</v>
+      </c>
+      <c r="U63" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="V63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A64" s="57"/>
+      <c r="B64" s="59">
+        <v>12</v>
+      </c>
+      <c r="C64" s="43">
+        <v>500</v>
+      </c>
+      <c r="H64" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I64" s="43">
+        <v>100</v>
+      </c>
+      <c r="J64" s="43">
+        <v>0</v>
+      </c>
+      <c r="K64" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L64" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M64" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N64" s="43">
+        <v>30</v>
+      </c>
+      <c r="O64" s="43">
+        <v>30</v>
+      </c>
+      <c r="P64" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q64" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R64" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S64" s="43">
+        <v>100</v>
+      </c>
+      <c r="T64">
+        <v>30</v>
+      </c>
+      <c r="U64" s="58">
+        <v>0.8</v>
+      </c>
+      <c r="V64" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A53:A64"/>
     <mergeCell ref="A49:A52"/>
     <mergeCell ref="A43:A48"/>
     <mergeCell ref="A38:A42"/>
@@ -17679,7 +18859,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -19189,7 +20369,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -19209,15 +20389,15 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="I1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
@@ -19239,18 +20419,18 @@
         <v>2.87647700605</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J2" s="55" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K2" s="55"/>
       <c r="L2" s="55" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M2" s="55"/>
       <c r="N2" s="55" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="O2" s="55"/>
     </row>
@@ -21426,15 +22606,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -21445,6 +22616,15 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21469,7 +22649,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -21498,7 +22678,7 @@
         <v>2.87824113329</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
@@ -36716,7 +37896,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -36739,7 +37919,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="32" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C2" s="32">
         <v>13.252202370437001</v>
@@ -38671,97 +39851,97 @@
   <sheetData>
     <row r="1" spans="1:49" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
       <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>31</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>32</v>
       </c>
-      <c r="S4" t="s">
-        <v>33</v>
-      </c>
       <c r="AC4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AD4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AI4" t="s">
         <v>63</v>
       </c>
-      <c r="AF4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>67</v>
-      </c>
       <c r="AJ4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AO4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AP4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AQ4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AR4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="AS4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AT4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="15.6" x14ac:dyDescent="0.3">
@@ -38828,7 +40008,7 @@
         <v>1.0042780206055512E-2</v>
       </c>
       <c r="AL5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AM5">
         <f>COUNT(AD5:AD54)</f>
@@ -38921,7 +40101,7 @@
         <v>9.9572197939444881E-3</v>
       </c>
       <c r="AL6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AM6">
         <f>AVERAGE(AD5:AD54)</f>
@@ -39014,7 +40194,7 @@
         <v>2.9957219793944487E-2</v>
       </c>
       <c r="AL7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AM7">
         <f>_xlfn.STDEV.S(AD5:AD54)</f>
@@ -39043,7 +40223,7 @@
         <v>4.9957219793944484E-2</v>
       </c>
       <c r="AV7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AW7">
         <f>MAX(AT5:AT54)</f>
@@ -39114,7 +40294,7 @@
         <v>6.223260863025018E-2</v>
       </c>
       <c r="AL8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AM8">
         <f>MAX(AJ5:AJ54)</f>
@@ -39143,7 +40323,7 @@
         <v>4.2232608630250176E-2</v>
       </c>
       <c r="AV8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AW8">
         <f>0.18845</f>
@@ -39300,7 +40480,7 @@
         <v>2.2232608630250172E-2</v>
       </c>
       <c r="AL10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AM10">
         <f>0.18845</f>
@@ -43115,14 +44295,14 @@
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" s="7">
         <f>AVERAGE(D5:D54)</f>
         <v>0.91610186017854023</v>
       </c>
       <c r="O55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P55" s="7">
         <f>AVERAGE(P5:P54)</f>
@@ -43131,14 +44311,14 @@
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56">
         <f>STDEV(D5:D54)</f>
         <v>0.26282524238527133</v>
       </c>
       <c r="O56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P56">
         <f>_xlfn.STDEV.S(P5:P54)</f>
@@ -43147,7 +44327,7 @@
     </row>
     <row r="57" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57">
         <f>SKEW(D5:D54)</f>
@@ -43156,60 +44336,60 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O60" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AC60" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" t="s">
         <v>25</v>
       </c>
-      <c r="E61" t="s">
-        <v>26</v>
-      </c>
       <c r="O61" t="s">
+        <v>29</v>
+      </c>
+      <c r="P61" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q61" t="s">
         <v>30</v>
       </c>
-      <c r="P61" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q61" t="s">
+      <c r="R61" t="s">
         <v>31</v>
       </c>
-      <c r="R61" t="s">
+      <c r="S61" t="s">
         <v>32</v>
       </c>
-      <c r="S61" t="s">
-        <v>33</v>
-      </c>
       <c r="AC61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AD61" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG61" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH61" t="s">
         <v>62</v>
       </c>
-      <c r="AE61" t="s">
+      <c r="AI61" t="s">
         <v>63</v>
       </c>
-      <c r="AF61" t="s">
+      <c r="AJ61" t="s">
         <v>64</v>
-      </c>
-      <c r="AG61" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH61" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI61" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ61" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.3">
@@ -43268,7 +44448,7 @@
         <v>1.3589932998991494E-2</v>
       </c>
       <c r="AL62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AM62">
         <f>COUNT(AD62:AD161)</f>
@@ -43331,7 +44511,7 @@
         <v>3.5899329989914942E-3</v>
       </c>
       <c r="AL63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AM63">
         <f>AVERAGE(AD62:AD161)</f>
@@ -43394,7 +44574,7 @@
         <v>6.410067001008506E-3</v>
       </c>
       <c r="AL64" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AM64">
         <f>_xlfn.STDEV.S(AD62:AD161)</f>
@@ -43457,7 +44637,7 @@
         <v>1.6410067001008506E-2</v>
       </c>
       <c r="AL65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AM65">
         <f>MAX(AJ62:AJ161)</f>
@@ -43576,7 +44756,7 @@
         <v>3.641006700100851E-2</v>
       </c>
       <c r="AL67" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AM67">
         <f>1.3581/SQRT(AM62)</f>
@@ -48853,14 +50033,14 @@
     </row>
     <row r="162" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C162" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D162" s="7">
         <f>AVERAGE(D62:D161)</f>
         <v>0.90449402464180051</v>
       </c>
       <c r="O162" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P162" s="7">
         <f>AVERAGE(P62:P161)</f>
@@ -48869,14 +50049,14 @@
     </row>
     <row r="163" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C163" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D163">
         <f>STDEV(D62:D161)</f>
         <v>0.27135102181909121</v>
       </c>
       <c r="O163" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P163">
         <f>STDEV(P62:P161)</f>
@@ -48885,7 +50065,7 @@
     </row>
     <row r="164" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D164">
         <f>SKEW(D62:D161)</f>
@@ -49422,7 +50602,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -51236,7 +52416,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -53704,7 +54884,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B103" s="32">
         <v>8.9024370000000008</v>
@@ -53727,7 +54907,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B104">
         <v>4.0611959999999998</v>
@@ -53750,7 +54930,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B105">
         <v>0.79597989999999996</v>
@@ -53773,7 +54953,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B106">
         <v>100</v>
@@ -53796,7 +54976,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -54704,7 +55884,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>
@@ -56873,7 +58053,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
updated evaluation scene for test 11
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB17531-AA3A-4179-ACA5-E284637CE27C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC94FB-D98F-471B-8A9A-EFF6D76CB94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
@@ -728,6 +728,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -762,21 +773,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -14629,10 +14629,10 @@
   <dimension ref="A1:Y64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T37" sqref="T37"/>
+      <selection pane="bottomRight" activeCell="V56" sqref="V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14730,7 +14730,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4">
@@ -14791,7 +14791,7 @@
         <f>N2</f>
         <v>3</v>
       </c>
-      <c r="U2" s="58">
+      <c r="U2" s="44">
         <v>0</v>
       </c>
       <c r="V2" t="s">
@@ -14799,7 +14799,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14858,7 +14858,7 @@
         <f t="shared" ref="T3:T60" si="1">N3</f>
         <v>10</v>
       </c>
-      <c r="U3" s="58">
+      <c r="U3" s="44">
         <v>0</v>
       </c>
       <c r="V3" t="s">
@@ -14866,7 +14866,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14925,7 +14925,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U4" s="58">
+      <c r="U4" s="44">
         <v>0</v>
       </c>
       <c r="V4" t="s">
@@ -14934,7 +14934,7 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -14993,7 +14993,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U5" s="58">
+      <c r="U5" s="44">
         <v>0</v>
       </c>
       <c r="V5" t="s">
@@ -15002,7 +15002,7 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -15062,7 +15062,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U6" s="58">
+      <c r="U6" s="44">
         <v>0</v>
       </c>
       <c r="V6" t="s">
@@ -15071,7 +15071,7 @@
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15131,7 +15131,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U7" s="58">
+      <c r="U7" s="44">
         <v>0</v>
       </c>
       <c r="V7" t="s">
@@ -15140,7 +15140,7 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -15197,7 +15197,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U8" s="58">
+      <c r="U8" s="44">
         <v>0</v>
       </c>
       <c r="V8" t="s">
@@ -15206,7 +15206,7 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="59" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5">
@@ -15268,7 +15268,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U9" s="58">
+      <c r="U9" s="44">
         <v>0</v>
       </c>
       <c r="V9" t="s">
@@ -15277,7 +15277,7 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -15337,7 +15337,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U10" s="58">
+      <c r="U10" s="44">
         <v>0</v>
       </c>
       <c r="V10" t="s">
@@ -15346,7 +15346,7 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -15406,7 +15406,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U11" s="58">
+      <c r="U11" s="44">
         <v>0</v>
       </c>
       <c r="V11" t="s">
@@ -15415,7 +15415,7 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -15475,7 +15475,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U12" s="58">
+      <c r="U12" s="44">
         <v>0</v>
       </c>
       <c r="V12" t="s">
@@ -15484,7 +15484,7 @@
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="55" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6">
@@ -15546,7 +15546,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U13" s="58">
+      <c r="U13" s="44">
         <v>0</v>
       </c>
       <c r="V13" t="s">
@@ -15554,7 +15554,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -15614,7 +15614,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U14" s="58">
+      <c r="U14" s="44">
         <v>0</v>
       </c>
       <c r="V14" t="s">
@@ -15622,7 +15622,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -15682,7 +15682,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U15" s="58">
+      <c r="U15" s="44">
         <v>0</v>
       </c>
       <c r="V15" t="s">
@@ -15690,7 +15690,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -15750,7 +15750,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U16" s="58">
+      <c r="U16" s="44">
         <v>0</v>
       </c>
       <c r="V16" t="s">
@@ -15758,7 +15758,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -15818,7 +15818,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U17" s="58">
+      <c r="U17" s="44">
         <v>0</v>
       </c>
       <c r="V17" t="s">
@@ -15826,7 +15826,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -15886,7 +15886,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U18" s="58">
+      <c r="U18" s="44">
         <v>0</v>
       </c>
       <c r="V18" t="s">
@@ -15956,7 +15956,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U19" s="58">
+      <c r="U19" s="44">
         <v>0</v>
       </c>
       <c r="V19" t="s">
@@ -15964,7 +15964,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="58" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16">
@@ -16026,7 +16026,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U20" s="58">
+      <c r="U20" s="44">
         <v>0</v>
       </c>
       <c r="V20" t="s">
@@ -16034,7 +16034,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="16">
         <v>2</v>
       </c>
@@ -16094,7 +16094,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U21" s="58">
+      <c r="U21" s="44">
         <v>0</v>
       </c>
       <c r="V21" t="s">
@@ -16102,7 +16102,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="56" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="10">
@@ -16164,7 +16164,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U22" s="58">
+      <c r="U22" s="44">
         <v>0</v>
       </c>
       <c r="V22" t="s">
@@ -16172,7 +16172,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -16232,7 +16232,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U23" s="58">
+      <c r="U23" s="44">
         <v>0</v>
       </c>
       <c r="V23" t="s">
@@ -16240,7 +16240,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -16300,7 +16300,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U24" s="58">
+      <c r="U24" s="44">
         <v>0</v>
       </c>
       <c r="V24" t="s">
@@ -16308,7 +16308,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -16368,7 +16368,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U25" s="58">
+      <c r="U25" s="44">
         <v>0</v>
       </c>
       <c r="V25" t="s">
@@ -16376,7 +16376,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -16436,7 +16436,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U26" s="58">
+      <c r="U26" s="44">
         <v>0</v>
       </c>
       <c r="V26" t="s">
@@ -16444,7 +16444,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="57" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="12">
@@ -16506,7 +16506,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U27" s="58">
+      <c r="U27" s="44">
         <v>0</v>
       </c>
       <c r="V27" t="s">
@@ -16514,7 +16514,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -16574,7 +16574,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U28" s="58">
+      <c r="U28" s="44">
         <v>0</v>
       </c>
       <c r="V28" t="s">
@@ -16582,7 +16582,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -16642,7 +16642,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U29" s="58">
+      <c r="U29" s="44">
         <v>0</v>
       </c>
       <c r="V29" t="s">
@@ -16650,7 +16650,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -16710,7 +16710,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U30" s="58">
+      <c r="U30" s="44">
         <v>0</v>
       </c>
       <c r="V30" t="s">
@@ -16718,7 +16718,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -16778,7 +16778,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U31" s="58">
+      <c r="U31" s="44">
         <v>0</v>
       </c>
       <c r="V31" t="s">
@@ -16786,7 +16786,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -16846,7 +16846,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U32" s="58">
+      <c r="U32" s="44">
         <v>0</v>
       </c>
       <c r="V32" t="s">
@@ -16854,7 +16854,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="52" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="14">
@@ -16916,7 +16916,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U33" s="58">
+      <c r="U33" s="44">
         <v>0</v>
       </c>
       <c r="V33" t="s">
@@ -16924,7 +16924,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="47"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -16984,7 +16984,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U34" s="58">
+      <c r="U34" s="44">
         <v>0</v>
       </c>
       <c r="V34" t="s">
@@ -16992,7 +16992,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="47"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -17052,7 +17052,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U35" s="58">
+      <c r="U35" s="44">
         <v>0</v>
       </c>
       <c r="V35" t="s">
@@ -17060,7 +17060,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="47"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -17120,7 +17120,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U36" s="58">
+      <c r="U36" s="44">
         <v>0</v>
       </c>
       <c r="V36" t="s">
@@ -17128,7 +17128,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="47"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -17188,7 +17188,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U37" s="58">
+      <c r="U37" s="44">
         <v>0</v>
       </c>
       <c r="V37" t="s">
@@ -17196,7 +17196,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="51" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="19">
@@ -17257,7 +17257,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U38" s="58">
+      <c r="U38" s="44">
         <v>0</v>
       </c>
       <c r="V38" t="s">
@@ -17265,7 +17265,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -17324,7 +17324,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U39" s="58">
+      <c r="U39" s="44">
         <v>0</v>
       </c>
       <c r="V39" t="s">
@@ -17332,7 +17332,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -17391,7 +17391,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U40" s="58">
+      <c r="U40" s="44">
         <v>0</v>
       </c>
       <c r="V40" t="s">
@@ -17399,7 +17399,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="46"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -17458,7 +17458,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U41" s="58">
+      <c r="U41" s="44">
         <v>0</v>
       </c>
       <c r="V41" t="s">
@@ -17466,7 +17466,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -17525,7 +17525,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U42" s="58">
+      <c r="U42" s="44">
         <v>0</v>
       </c>
       <c r="V42" t="s">
@@ -17533,7 +17533,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="50" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="23">
@@ -17595,7 +17595,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U43" s="58">
+      <c r="U43" s="44">
         <v>0</v>
       </c>
       <c r="V43" t="s">
@@ -17603,7 +17603,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -17663,7 +17663,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U44" s="58">
+      <c r="U44" s="44">
         <v>0</v>
       </c>
       <c r="V44" t="s">
@@ -17671,7 +17671,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -17731,7 +17731,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U45" s="58">
+      <c r="U45" s="44">
         <v>0</v>
       </c>
       <c r="V45" t="s">
@@ -17739,7 +17739,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -17799,7 +17799,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U46" s="58">
+      <c r="U46" s="44">
         <v>0</v>
       </c>
       <c r="V46" t="s">
@@ -17807,7 +17807,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -17867,7 +17867,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U47" s="58">
+      <c r="U47" s="44">
         <v>0</v>
       </c>
       <c r="V47" t="s">
@@ -17875,7 +17875,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="45"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -17932,7 +17932,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U48" s="58">
+      <c r="U48" s="44">
         <v>0</v>
       </c>
       <c r="V48" t="s">
@@ -17940,7 +17940,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="44" t="s">
+      <c r="A49" s="49" t="s">
         <v>85</v>
       </c>
       <c r="B49" s="23">
@@ -17993,7 +17993,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="U49" s="58">
+      <c r="U49" s="44">
         <v>0</v>
       </c>
       <c r="V49" t="s">
@@ -18001,7 +18001,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="44"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="23">
         <v>2</v>
       </c>
@@ -18048,7 +18048,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U50" s="58">
+      <c r="U50" s="44">
         <v>0</v>
       </c>
       <c r="V50" t="s">
@@ -18056,7 +18056,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="44"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="23">
         <v>3</v>
       </c>
@@ -18103,7 +18103,7 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="U51" s="58">
+      <c r="U51" s="44">
         <v>0</v>
       </c>
       <c r="V51" t="s">
@@ -18111,7 +18111,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="44"/>
+      <c r="A52" s="49"/>
       <c r="B52" s="23">
         <v>4</v>
       </c>
@@ -18154,11 +18154,11 @@
       <c r="S52" s="37">
         <v>100</v>
       </c>
-      <c r="T52" s="61" t="str">
+      <c r="T52" s="47" t="str">
         <f t="shared" si="1"/>
         <v>Max</v>
       </c>
-      <c r="U52" s="58">
+      <c r="U52" s="44">
         <v>0</v>
       </c>
       <c r="V52" t="s">
@@ -18166,16 +18166,16 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="59">
+      <c r="B53" s="45">
         <v>1</v>
       </c>
       <c r="C53" s="43">
         <v>500</v>
       </c>
-      <c r="H53" s="60" t="s">
+      <c r="H53" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I53" s="43">
@@ -18215,7 +18215,7 @@
         <f>N53*0.3</f>
         <v>9</v>
       </c>
-      <c r="U53" s="58">
+      <c r="U53" s="44">
         <v>0.3</v>
       </c>
       <c r="V53" t="s">
@@ -18223,14 +18223,14 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="57"/>
-      <c r="B54" s="59">
+      <c r="A54" s="48"/>
+      <c r="B54" s="45">
         <v>2</v>
       </c>
       <c r="C54" s="43">
         <v>500</v>
       </c>
-      <c r="H54" s="60" t="s">
+      <c r="H54" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I54" s="43">
@@ -18270,7 +18270,7 @@
         <f>N54*0.5</f>
         <v>15</v>
       </c>
-      <c r="U54" s="58">
+      <c r="U54" s="44">
         <v>0.3</v>
       </c>
       <c r="V54" t="s">
@@ -18278,14 +18278,14 @@
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="57"/>
-      <c r="B55" s="59">
+      <c r="A55" s="48"/>
+      <c r="B55" s="45">
         <v>3</v>
       </c>
       <c r="C55" s="43">
         <v>500</v>
       </c>
-      <c r="H55" s="60" t="s">
+      <c r="H55" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I55" s="43">
@@ -18325,7 +18325,7 @@
         <f>N55*0.8</f>
         <v>24</v>
       </c>
-      <c r="U55" s="58">
+      <c r="U55" s="44">
         <v>0.3</v>
       </c>
       <c r="V55" t="s">
@@ -18333,8 +18333,8 @@
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="57"/>
-      <c r="B56" s="59">
+      <c r="A56" s="48"/>
+      <c r="B56" s="45">
         <v>4</v>
       </c>
       <c r="C56" s="43">
@@ -18342,7 +18342,7 @@
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
-      <c r="H56" s="60" t="s">
+      <c r="H56" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I56" s="43">
@@ -18382,7 +18382,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="U56" s="58">
+      <c r="U56" s="44">
         <v>0.3</v>
       </c>
       <c r="V56" t="s">
@@ -18390,14 +18390,14 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="57"/>
-      <c r="B57" s="59">
+      <c r="A57" s="48"/>
+      <c r="B57" s="45">
         <v>5</v>
       </c>
       <c r="C57" s="43">
         <v>500</v>
       </c>
-      <c r="H57" s="60" t="s">
+      <c r="H57" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I57" s="43">
@@ -18437,7 +18437,7 @@
         <f>N57*0.3</f>
         <v>9</v>
       </c>
-      <c r="U57" s="58">
+      <c r="U57" s="44">
         <v>0.5</v>
       </c>
       <c r="V57" t="s">
@@ -18445,14 +18445,14 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="57"/>
-      <c r="B58" s="59">
+      <c r="A58" s="48"/>
+      <c r="B58" s="45">
         <v>6</v>
       </c>
       <c r="C58" s="43">
         <v>500</v>
       </c>
-      <c r="H58" s="60" t="s">
+      <c r="H58" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I58" s="43">
@@ -18492,7 +18492,7 @@
         <f>N58*0.5</f>
         <v>15</v>
       </c>
-      <c r="U58" s="58">
+      <c r="U58" s="44">
         <v>0.5</v>
       </c>
       <c r="V58" t="s">
@@ -18500,14 +18500,14 @@
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="57"/>
-      <c r="B59" s="59">
+      <c r="A59" s="48"/>
+      <c r="B59" s="45">
         <v>7</v>
       </c>
       <c r="C59" s="43">
         <v>500</v>
       </c>
-      <c r="H59" s="60" t="s">
+      <c r="H59" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I59" s="43">
@@ -18547,7 +18547,7 @@
         <f>N59*0.8</f>
         <v>24</v>
       </c>
-      <c r="U59" s="58">
+      <c r="U59" s="44">
         <v>0.5</v>
       </c>
       <c r="V59" t="s">
@@ -18555,14 +18555,14 @@
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="57"/>
-      <c r="B60" s="59">
+      <c r="A60" s="48"/>
+      <c r="B60" s="45">
         <v>8</v>
       </c>
       <c r="C60" s="43">
         <v>500</v>
       </c>
-      <c r="H60" s="60" t="s">
+      <c r="H60" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I60" s="43">
@@ -18602,7 +18602,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="U60" s="58">
+      <c r="U60" s="44">
         <v>0.5</v>
       </c>
       <c r="V60" t="s">
@@ -18610,14 +18610,14 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="57"/>
-      <c r="B61" s="59">
+      <c r="A61" s="48"/>
+      <c r="B61" s="45">
         <v>9</v>
       </c>
       <c r="C61" s="43">
         <v>500</v>
       </c>
-      <c r="H61" s="60" t="s">
+      <c r="H61" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I61" s="43">
@@ -18656,7 +18656,7 @@
       <c r="T61">
         <v>9</v>
       </c>
-      <c r="U61" s="58">
+      <c r="U61" s="44">
         <v>0.8</v>
       </c>
       <c r="V61" t="s">
@@ -18664,14 +18664,14 @@
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="57"/>
-      <c r="B62" s="59">
+      <c r="A62" s="48"/>
+      <c r="B62" s="45">
         <v>10</v>
       </c>
       <c r="C62" s="43">
         <v>500</v>
       </c>
-      <c r="H62" s="60" t="s">
+      <c r="H62" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I62" s="43">
@@ -18710,7 +18710,7 @@
       <c r="T62">
         <v>15</v>
       </c>
-      <c r="U62" s="58">
+      <c r="U62" s="44">
         <v>0.8</v>
       </c>
       <c r="V62" t="s">
@@ -18718,14 +18718,14 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="57"/>
-      <c r="B63" s="59">
+      <c r="A63" s="48"/>
+      <c r="B63" s="45">
         <v>11</v>
       </c>
       <c r="C63" s="43">
         <v>500</v>
       </c>
-      <c r="H63" s="60" t="s">
+      <c r="H63" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I63" s="43">
@@ -18764,7 +18764,7 @@
       <c r="T63">
         <v>24</v>
       </c>
-      <c r="U63" s="58">
+      <c r="U63" s="44">
         <v>0.8</v>
       </c>
       <c r="V63" t="s">
@@ -18772,14 +18772,14 @@
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="57"/>
-      <c r="B64" s="59">
+      <c r="A64" s="48"/>
+      <c r="B64" s="45">
         <v>12</v>
       </c>
       <c r="C64" s="43">
         <v>500</v>
       </c>
-      <c r="H64" s="60" t="s">
+      <c r="H64" s="46" t="s">
         <v>103</v>
       </c>
       <c r="I64" s="43">
@@ -18818,7 +18818,7 @@
       <c r="T64">
         <v>30</v>
       </c>
-      <c r="U64" s="58">
+      <c r="U64" s="44">
         <v>0.8</v>
       </c>
       <c r="V64" t="s">
@@ -18827,17 +18827,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A53:A64"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A33:A37"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A53:A64"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20389,15 +20389,15 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
@@ -20421,18 +20421,18 @@
       <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55" t="s">
+      <c r="K2" s="61"/>
+      <c r="L2" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55" t="s">
+      <c r="M2" s="61"/>
+      <c r="N2" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="55"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
@@ -20459,18 +20459,18 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="61">
         <v>1.2</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55">
+      <c r="K3" s="61"/>
+      <c r="L3" s="61">
         <v>3</v>
       </c>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55">
+      <c r="M3" s="61"/>
+      <c r="N3" s="61">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="55"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
@@ -20497,18 +20497,18 @@
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="J4" s="55">
+      <c r="J4" s="61">
         <v>1.3</v>
       </c>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55">
+      <c r="K4" s="61"/>
+      <c r="L4" s="61">
         <v>4</v>
       </c>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="55"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
@@ -20535,18 +20535,18 @@
       <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="61">
         <v>2.36</v>
       </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55">
+      <c r="K5" s="61"/>
+      <c r="L5" s="61">
         <v>6</v>
       </c>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55">
+      <c r="M5" s="61"/>
+      <c r="N5" s="61">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="55"/>
+      <c r="O5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -20573,18 +20573,18 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J6" s="61">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55">
+      <c r="K6" s="61"/>
+      <c r="L6" s="61">
         <v>8</v>
       </c>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55">
+      <c r="M6" s="61"/>
+      <c r="N6" s="61">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="55"/>
+      <c r="O6" s="61"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
@@ -20611,18 +20611,18 @@
       <c r="I7">
         <v>1000</v>
       </c>
-      <c r="J7" s="55">
+      <c r="J7" s="61">
         <v>3.55</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55">
+      <c r="K7" s="61"/>
+      <c r="L7" s="61">
         <v>12</v>
       </c>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55">
+      <c r="M7" s="61"/>
+      <c r="N7" s="61">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="55"/>
+      <c r="O7" s="61"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
@@ -22606,6 +22606,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -22616,15 +22625,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22677,12 +22677,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">

</xml_diff>

<commit_message>
updated simulation configurations for set11 (transacion limit)
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC94FB-D98F-471B-8A9A-EFF6D76CB94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2BB6B-2280-4A25-99CC-84C3DD1211A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Set8" sheetId="10" r:id="rId8"/>
     <sheet name="Set9" sheetId="11" r:id="rId9"/>
     <sheet name="Set10" sheetId="12" r:id="rId10"/>
+    <sheet name="Set11" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="104">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -341,9 +342,6 @@
     <t>inf</t>
   </si>
   <si>
-    <t>1000s</t>
-  </si>
-  <si>
     <t>Number Of Anonymizer</t>
   </si>
   <si>
@@ -359,9 +357,6 @@
     <t>Probability Evil Anonimizer</t>
   </si>
   <si>
-    <t>Sim Time</t>
-  </si>
-  <si>
     <t>Anonymizer Life Time</t>
   </si>
   <si>
@@ -369,6 +364,9 @@
   </si>
   <si>
     <t>Anonymizer Dissemination Time</t>
+  </si>
+  <si>
+    <t>Transaction Limiter</t>
   </si>
 </sst>
 </file>
@@ -486,7 +484,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,6 +548,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -639,7 +643,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -654,8 +658,9 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,21 +741,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -772,14 +762,33 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="12" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
+    <cellStyle name="40% - Accent2" xfId="14" builtinId="35"/>
     <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="12" builtinId="36"/>
@@ -14628,11 +14637,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q37" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V56" sqref="V56"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14657,7 +14666,7 @@
     <col min="19" max="19" width="22.33203125" customWidth="1"/>
     <col min="20" max="20" width="34.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14702,35 +14711,35 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="Q1" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="V1" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4">
@@ -14799,7 +14808,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14866,7 +14875,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14934,7 +14943,7 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -15002,7 +15011,7 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -15071,7 +15080,7 @@
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15140,7 +15149,7 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -15206,7 +15215,7 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="54" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5">
@@ -15277,7 +15286,7 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -15346,7 +15355,7 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -15415,7 +15424,7 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -15484,7 +15493,7 @@
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="50" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6">
@@ -15554,7 +15563,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -15622,7 +15631,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -15690,7 +15699,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -15758,7 +15767,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -15826,7 +15835,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -15964,7 +15973,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="53" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16">
@@ -16034,7 +16043,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="16">
         <v>2</v>
       </c>
@@ -16102,7 +16111,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="51" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="10">
@@ -16172,7 +16181,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -16240,7 +16249,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="56"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -16308,7 +16317,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -16376,7 +16385,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -16444,7 +16453,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="12">
@@ -16514,7 +16523,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -16582,7 +16591,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -16650,7 +16659,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -16718,7 +16727,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -16786,7 +16795,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -16854,7 +16863,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="59" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="14">
@@ -16924,7 +16933,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -16992,7 +17001,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -17060,7 +17069,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="52"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -17128,7 +17137,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="52"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -17196,7 +17205,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="58" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="19">
@@ -17265,7 +17274,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
+      <c r="A39" s="58"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -17332,7 +17341,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="51"/>
+      <c r="A40" s="58"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -17399,7 +17408,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="51"/>
+      <c r="A41" s="58"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -17466,7 +17475,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="51"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -17533,7 +17542,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="57" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="23">
@@ -17603,7 +17612,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="50"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -17671,7 +17680,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="50"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -17739,7 +17748,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -17807,7 +17816,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="50"/>
+      <c r="A47" s="57"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -17875,7 +17884,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
+      <c r="A48" s="57"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -17940,7 +17949,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="56" t="s">
         <v>85</v>
       </c>
       <c r="B49" s="23">
@@ -18001,7 +18010,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="49"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="23">
         <v>2</v>
       </c>
@@ -18056,7 +18065,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="49"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="23">
         <v>3</v>
       </c>
@@ -18111,7 +18120,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="49"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="23">
         <v>4</v>
       </c>
@@ -18166,7 +18175,7 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="55" t="s">
         <v>93</v>
       </c>
       <c r="B53" s="45">
@@ -18176,7 +18185,7 @@
         <v>500</v>
       </c>
       <c r="H53" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I53" s="43">
         <v>100</v>
@@ -18218,12 +18227,12 @@
       <c r="U53" s="44">
         <v>0.3</v>
       </c>
-      <c r="V53" t="s">
-        <v>95</v>
+      <c r="V53">
+        <v>10000</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="48"/>
+      <c r="A54" s="55"/>
       <c r="B54" s="45">
         <v>2</v>
       </c>
@@ -18231,7 +18240,7 @@
         <v>500</v>
       </c>
       <c r="H54" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I54" s="43">
         <v>100</v>
@@ -18273,12 +18282,12 @@
       <c r="U54" s="44">
         <v>0.3</v>
       </c>
-      <c r="V54" t="s">
-        <v>95</v>
+      <c r="V54">
+        <v>10000</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="48"/>
+      <c r="A55" s="55"/>
       <c r="B55" s="45">
         <v>3</v>
       </c>
@@ -18286,7 +18295,7 @@
         <v>500</v>
       </c>
       <c r="H55" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I55" s="43">
         <v>100</v>
@@ -18328,12 +18337,12 @@
       <c r="U55" s="44">
         <v>0.3</v>
       </c>
-      <c r="V55" t="s">
-        <v>95</v>
+      <c r="V55">
+        <v>10000</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="48"/>
+      <c r="A56" s="55"/>
       <c r="B56" s="45">
         <v>4</v>
       </c>
@@ -18343,7 +18352,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I56" s="43">
         <v>100</v>
@@ -18385,12 +18394,12 @@
       <c r="U56" s="44">
         <v>0.3</v>
       </c>
-      <c r="V56" t="s">
-        <v>95</v>
+      <c r="V56">
+        <v>10000</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="48"/>
+      <c r="A57" s="55"/>
       <c r="B57" s="45">
         <v>5</v>
       </c>
@@ -18398,7 +18407,7 @@
         <v>500</v>
       </c>
       <c r="H57" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I57" s="43">
         <v>100</v>
@@ -18440,12 +18449,12 @@
       <c r="U57" s="44">
         <v>0.5</v>
       </c>
-      <c r="V57" t="s">
-        <v>95</v>
+      <c r="V57">
+        <v>10000</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="48"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="45">
         <v>6</v>
       </c>
@@ -18453,7 +18462,7 @@
         <v>500</v>
       </c>
       <c r="H58" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I58" s="43">
         <v>100</v>
@@ -18495,12 +18504,12 @@
       <c r="U58" s="44">
         <v>0.5</v>
       </c>
-      <c r="V58" t="s">
-        <v>95</v>
+      <c r="V58">
+        <v>10000</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="48"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="45">
         <v>7</v>
       </c>
@@ -18508,7 +18517,7 @@
         <v>500</v>
       </c>
       <c r="H59" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I59" s="43">
         <v>100</v>
@@ -18550,12 +18559,12 @@
       <c r="U59" s="44">
         <v>0.5</v>
       </c>
-      <c r="V59" t="s">
-        <v>95</v>
+      <c r="V59">
+        <v>10000</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="48"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="45">
         <v>8</v>
       </c>
@@ -18563,7 +18572,7 @@
         <v>500</v>
       </c>
       <c r="H60" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I60" s="43">
         <v>100</v>
@@ -18605,12 +18614,12 @@
       <c r="U60" s="44">
         <v>0.5</v>
       </c>
-      <c r="V60" t="s">
-        <v>95</v>
+      <c r="V60">
+        <v>10000</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="48"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="45">
         <v>9</v>
       </c>
@@ -18618,7 +18627,7 @@
         <v>500</v>
       </c>
       <c r="H61" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I61" s="43">
         <v>100</v>
@@ -18659,12 +18668,12 @@
       <c r="U61" s="44">
         <v>0.8</v>
       </c>
-      <c r="V61" t="s">
-        <v>95</v>
+      <c r="V61">
+        <v>10000</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="48"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="45">
         <v>10</v>
       </c>
@@ -18672,7 +18681,7 @@
         <v>500</v>
       </c>
       <c r="H62" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I62" s="43">
         <v>100</v>
@@ -18713,12 +18722,12 @@
       <c r="U62" s="44">
         <v>0.8</v>
       </c>
-      <c r="V62" t="s">
-        <v>95</v>
+      <c r="V62">
+        <v>10000</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="48"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="45">
         <v>11</v>
       </c>
@@ -18726,7 +18735,7 @@
         <v>500</v>
       </c>
       <c r="H63" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I63" s="43">
         <v>100</v>
@@ -18767,12 +18776,12 @@
       <c r="U63" s="44">
         <v>0.8</v>
       </c>
-      <c r="V63" t="s">
-        <v>95</v>
+      <c r="V63">
+        <v>10000</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="48"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="45">
         <v>12</v>
       </c>
@@ -18780,7 +18789,7 @@
         <v>500</v>
       </c>
       <c r="H64" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I64" s="43">
         <v>100</v>
@@ -18821,23 +18830,23 @@
       <c r="U64" s="44">
         <v>0.8</v>
       </c>
-      <c r="V64" t="s">
-        <v>95</v>
+      <c r="V64">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A53:A64"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A33:A37"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A53:A64"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20350,12 +20359,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03224E0E-0471-4EB9-BE20-7A75388FABD1}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="63">
+        <v>1</v>
+      </c>
+      <c r="C1" s="63">
+        <v>2</v>
+      </c>
+      <c r="D1" s="63">
+        <v>3</v>
+      </c>
+      <c r="E1" s="63">
+        <v>4</v>
+      </c>
+      <c r="F1" s="62">
+        <v>5</v>
+      </c>
+      <c r="G1" s="62">
+        <v>6</v>
+      </c>
+      <c r="H1" s="62">
+        <v>7</v>
+      </c>
+      <c r="I1" s="62">
+        <v>8</v>
+      </c>
+      <c r="J1" s="64">
+        <v>9</v>
+      </c>
+      <c r="K1" s="64">
+        <v>10</v>
+      </c>
+      <c r="L1" s="64">
+        <v>11</v>
+      </c>
+      <c r="M1" s="64">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20389,15 +20457,15 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
@@ -20421,18 +20489,18 @@
       <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61" t="s">
+      <c r="K2" s="60"/>
+      <c r="L2" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61" t="s">
+      <c r="M2" s="60"/>
+      <c r="N2" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="61"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
@@ -20459,18 +20527,18 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="61">
+      <c r="J3" s="60">
         <v>1.2</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61">
+      <c r="K3" s="60"/>
+      <c r="L3" s="60">
         <v>3</v>
       </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61">
+      <c r="M3" s="60"/>
+      <c r="N3" s="60">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="61"/>
+      <c r="O3" s="60"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
@@ -20497,18 +20565,18 @@
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="J4" s="61">
+      <c r="J4" s="60">
         <v>1.3</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61">
+      <c r="K4" s="60"/>
+      <c r="L4" s="60">
         <v>4</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="61"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
@@ -20535,18 +20603,18 @@
       <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5" s="61">
+      <c r="J5" s="60">
         <v>2.36</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61">
+      <c r="K5" s="60"/>
+      <c r="L5" s="60">
         <v>6</v>
       </c>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61">
+      <c r="M5" s="60"/>
+      <c r="N5" s="60">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="61"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -20573,18 +20641,18 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" s="61">
+      <c r="J6" s="60">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61">
+      <c r="K6" s="60"/>
+      <c r="L6" s="60">
         <v>8</v>
       </c>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61">
+      <c r="M6" s="60"/>
+      <c r="N6" s="60">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="61"/>
+      <c r="O6" s="60"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
@@ -20611,18 +20679,18 @@
       <c r="I7">
         <v>1000</v>
       </c>
-      <c r="J7" s="61">
+      <c r="J7" s="60">
         <v>3.55</v>
       </c>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61">
+      <c r="K7" s="60"/>
+      <c r="L7" s="60">
         <v>12</v>
       </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61">
+      <c r="M7" s="60"/>
+      <c r="N7" s="60">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="61"/>
+      <c r="O7" s="60"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
@@ -22606,15 +22674,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -22625,6 +22684,15 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22677,12 +22745,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">

</xml_diff>

<commit_message>
updated simulation set11 with 5% evil nodes
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2BB6B-2280-4A25-99CC-84C3DD1211A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE75DDB-6B11-4038-A964-3C99A1F5FDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="106">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -342,41 +342,48 @@
     <t>inf</t>
   </si>
   <si>
-    <t>Number Of Anonymizer</t>
-  </si>
-  <si>
-    <t>Anonymus Auditing Timeout Time</t>
-  </si>
-  <si>
     <t>Transaction Timeout Time</t>
-  </si>
-  <si>
-    <t>Anonimizer Number Threshold</t>
-  </si>
-  <si>
-    <t>Probability Evil Anonimizer</t>
-  </si>
-  <si>
-    <t>Anonymizer Life Time</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Anonymizer Dissemination Time</t>
+    <t>Transaction Limiter</t>
   </si>
   <si>
-    <t>Transaction Limiter</t>
+    <t>* 11 - Evil Anonimizer</t>
+  </si>
+  <si>
+    <t>* 10 - Variation of Anonymizer nodes</t>
+  </si>
+  <si>
+    <t>* Number Of Anonymizer</t>
+  </si>
+  <si>
+    <t>* Anonymus Auditing Timeout Time</t>
+  </si>
+  <si>
+    <t>* Anonymizer Dissemination Time</t>
+  </si>
+  <si>
+    <t>* Anonymizer Life Time</t>
+  </si>
+  <si>
+    <t>* Anonimizer Number Threshold</t>
+  </si>
+  <si>
+    <t>* Probability Evil Anonimizer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.000000000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -484,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,12 +560,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -642,8 +653,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -658,9 +684,11 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -741,6 +769,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -783,18 +818,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="14" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="9" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="15"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="16" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
-    <cellStyle name="40% - Accent2" xfId="14" builtinId="35"/>
+  <cellStyles count="17">
     <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="12" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -802,7 +836,9 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10"/>
     <cellStyle name="Output" xfId="10" builtinId="21"/>
+    <cellStyle name="Percent" xfId="14" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -14635,18 +14671,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A53" sqref="A53:A64"/>
+      <selection pane="bottomRight" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" style="13" customWidth="1"/>
     <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.33203125" hidden="1" customWidth="1"/>
@@ -14658,14 +14694,14 @@
     <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.5546875" customWidth="1"/>
     <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.109375" customWidth="1"/>
   </cols>
@@ -14711,35 +14747,35 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>102</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4">
@@ -14808,7 +14844,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14875,7 +14911,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14943,7 +14979,7 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -15011,7 +15047,7 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -15080,7 +15116,7 @@
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15149,7 +15185,7 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -15215,7 +15251,7 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="59" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5">
@@ -15286,7 +15322,7 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -15355,7 +15391,7 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -15424,7 +15460,7 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -15493,7 +15529,7 @@
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="55" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6">
@@ -15563,7 +15599,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -15631,7 +15667,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -15699,7 +15735,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -15767,7 +15803,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -15835,7 +15871,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -15973,7 +16009,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="58" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16">
@@ -16043,7 +16079,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="16">
         <v>2</v>
       </c>
@@ -16111,7 +16147,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="56" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="10">
@@ -16181,7 +16217,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -16249,7 +16285,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -16317,7 +16353,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -16385,7 +16421,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -16453,7 +16489,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="57" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="12">
@@ -16523,7 +16559,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -16591,7 +16627,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -16659,7 +16695,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -16727,7 +16763,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -16795,7 +16831,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -16863,7 +16899,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="64" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="14">
@@ -16933,7 +16969,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -17001,7 +17037,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="59"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -17069,7 +17105,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="59"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -17137,7 +17173,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="59"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -17205,7 +17241,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="63" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="19">
@@ -17274,7 +17310,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="58"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -17341,7 +17377,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="58"/>
+      <c r="A40" s="63"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -17408,7 +17444,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="58"/>
+      <c r="A41" s="63"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -17475,7 +17511,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="58"/>
+      <c r="A42" s="63"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -17542,7 +17578,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="62" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="23">
@@ -17612,7 +17648,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="57"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -17680,7 +17716,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="57"/>
+      <c r="A45" s="62"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -17748,7 +17784,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="57"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -17816,7 +17852,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="57"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -17884,7 +17920,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="57"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -17949,8 +17985,8 @@
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="56" t="s">
-        <v>85</v>
+      <c r="A49" s="61" t="s">
+        <v>99</v>
       </c>
       <c r="B49" s="23">
         <v>1</v>
@@ -18010,7 +18046,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="56"/>
+      <c r="A50" s="61"/>
       <c r="B50" s="23">
         <v>2</v>
       </c>
@@ -18065,7 +18101,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="56"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="23">
         <v>3</v>
       </c>
@@ -18120,7 +18156,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="56"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="23">
         <v>4</v>
       </c>
@@ -18175,8 +18211,8 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="55" t="s">
-        <v>93</v>
+      <c r="A53" s="60" t="s">
+        <v>98</v>
       </c>
       <c r="B53" s="45">
         <v>1</v>
@@ -18185,7 +18221,7 @@
         <v>500</v>
       </c>
       <c r="H53" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I53" s="43">
         <v>100</v>
@@ -18225,14 +18261,14 @@
         <v>9</v>
       </c>
       <c r="U53" s="44">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="V53">
         <v>10000</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="55"/>
+      <c r="A54" s="60"/>
       <c r="B54" s="45">
         <v>2</v>
       </c>
@@ -18240,7 +18276,7 @@
         <v>500</v>
       </c>
       <c r="H54" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I54" s="43">
         <v>100</v>
@@ -18280,14 +18316,14 @@
         <v>15</v>
       </c>
       <c r="U54" s="44">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="V54">
         <v>10000</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="55"/>
+      <c r="A55" s="60"/>
       <c r="B55" s="45">
         <v>3</v>
       </c>
@@ -18295,7 +18331,7 @@
         <v>500</v>
       </c>
       <c r="H55" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I55" s="43">
         <v>100</v>
@@ -18335,14 +18371,14 @@
         <v>24</v>
       </c>
       <c r="U55" s="44">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="V55">
         <v>10000</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="55"/>
+      <c r="A56" s="60"/>
       <c r="B56" s="45">
         <v>4</v>
       </c>
@@ -18352,7 +18388,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I56" s="43">
         <v>100</v>
@@ -18392,14 +18428,14 @@
         <v>30</v>
       </c>
       <c r="U56" s="44">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="V56">
         <v>10000</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="55"/>
+      <c r="A57" s="60"/>
       <c r="B57" s="45">
         <v>5</v>
       </c>
@@ -18407,7 +18443,7 @@
         <v>500</v>
       </c>
       <c r="H57" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I57" s="43">
         <v>100</v>
@@ -18447,14 +18483,14 @@
         <v>9</v>
       </c>
       <c r="U57" s="44">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="V57">
         <v>10000</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="55"/>
+      <c r="A58" s="60"/>
       <c r="B58" s="45">
         <v>6</v>
       </c>
@@ -18462,7 +18498,7 @@
         <v>500</v>
       </c>
       <c r="H58" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I58" s="43">
         <v>100</v>
@@ -18502,14 +18538,14 @@
         <v>15</v>
       </c>
       <c r="U58" s="44">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="V58">
         <v>10000</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="55"/>
+      <c r="A59" s="60"/>
       <c r="B59" s="45">
         <v>7</v>
       </c>
@@ -18517,7 +18553,7 @@
         <v>500</v>
       </c>
       <c r="H59" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I59" s="43">
         <v>100</v>
@@ -18557,14 +18593,14 @@
         <v>24</v>
       </c>
       <c r="U59" s="44">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="V59">
         <v>10000</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="55"/>
+      <c r="A60" s="60"/>
       <c r="B60" s="45">
         <v>8</v>
       </c>
@@ -18572,7 +18608,7 @@
         <v>500</v>
       </c>
       <c r="H60" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I60" s="43">
         <v>100</v>
@@ -18612,14 +18648,14 @@
         <v>30</v>
       </c>
       <c r="U60" s="44">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="V60">
         <v>10000</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="55"/>
+      <c r="A61" s="60"/>
       <c r="B61" s="45">
         <v>9</v>
       </c>
@@ -18627,7 +18663,7 @@
         <v>500</v>
       </c>
       <c r="H61" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I61" s="43">
         <v>100</v>
@@ -18666,14 +18702,14 @@
         <v>9</v>
       </c>
       <c r="U61" s="44">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="V61">
         <v>10000</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="55"/>
+      <c r="A62" s="60"/>
       <c r="B62" s="45">
         <v>10</v>
       </c>
@@ -18681,7 +18717,7 @@
         <v>500</v>
       </c>
       <c r="H62" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I62" s="43">
         <v>100</v>
@@ -18720,14 +18756,14 @@
         <v>15</v>
       </c>
       <c r="U62" s="44">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="V62">
         <v>10000</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="55"/>
+      <c r="A63" s="60"/>
       <c r="B63" s="45">
         <v>11</v>
       </c>
@@ -18735,7 +18771,7 @@
         <v>500</v>
       </c>
       <c r="H63" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I63" s="43">
         <v>100</v>
@@ -18774,14 +18810,14 @@
         <v>24</v>
       </c>
       <c r="U63" s="44">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="V63">
         <v>10000</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="55"/>
+      <c r="A64" s="60"/>
       <c r="B64" s="45">
         <v>12</v>
       </c>
@@ -18789,7 +18825,7 @@
         <v>500</v>
       </c>
       <c r="H64" s="46" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I64" s="43">
         <v>100</v>
@@ -18828,19 +18864,235 @@
         <v>30</v>
       </c>
       <c r="U64" s="44">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="V64">
         <v>10000</v>
       </c>
     </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A65" s="60"/>
+      <c r="B65" s="45">
+        <v>13</v>
+      </c>
+      <c r="C65" s="50">
+        <v>500</v>
+      </c>
+      <c r="H65" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I65" s="50">
+        <v>100</v>
+      </c>
+      <c r="J65" s="50">
+        <v>0</v>
+      </c>
+      <c r="K65" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L65" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M65" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="N65" s="50">
+        <v>30</v>
+      </c>
+      <c r="O65" s="50">
+        <v>30</v>
+      </c>
+      <c r="P65" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q65" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="R65" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="S65" s="50">
+        <v>100</v>
+      </c>
+      <c r="T65">
+        <v>9</v>
+      </c>
+      <c r="U65" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="V65">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A66" s="60"/>
+      <c r="B66" s="45">
+        <v>14</v>
+      </c>
+      <c r="C66" s="50">
+        <v>500</v>
+      </c>
+      <c r="H66" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I66" s="50">
+        <v>100</v>
+      </c>
+      <c r="J66" s="50">
+        <v>0</v>
+      </c>
+      <c r="K66" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L66" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M66" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="N66" s="50">
+        <v>30</v>
+      </c>
+      <c r="O66" s="50">
+        <v>30</v>
+      </c>
+      <c r="P66" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q66" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="R66" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="S66" s="50">
+        <v>100</v>
+      </c>
+      <c r="T66">
+        <v>15</v>
+      </c>
+      <c r="U66" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="V66">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A67" s="60"/>
+      <c r="B67" s="45">
+        <v>15</v>
+      </c>
+      <c r="C67" s="50">
+        <v>500</v>
+      </c>
+      <c r="H67" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I67" s="50">
+        <v>100</v>
+      </c>
+      <c r="J67" s="50">
+        <v>0</v>
+      </c>
+      <c r="K67" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L67" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M67" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="N67" s="50">
+        <v>30</v>
+      </c>
+      <c r="O67" s="50">
+        <v>30</v>
+      </c>
+      <c r="P67" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q67" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="R67" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="S67" s="50">
+        <v>100</v>
+      </c>
+      <c r="T67">
+        <v>24</v>
+      </c>
+      <c r="U67" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="V67">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A68" s="60"/>
+      <c r="B68" s="45">
+        <v>16</v>
+      </c>
+      <c r="C68" s="50">
+        <v>500</v>
+      </c>
+      <c r="H68" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I68" s="50">
+        <v>100</v>
+      </c>
+      <c r="J68" s="50">
+        <v>0</v>
+      </c>
+      <c r="K68" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L68" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M68" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="N68" s="50">
+        <v>30</v>
+      </c>
+      <c r="O68" s="50">
+        <v>30</v>
+      </c>
+      <c r="P68" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q68" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="R68" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="S68" s="50">
+        <v>100</v>
+      </c>
+      <c r="T68">
+        <v>30</v>
+      </c>
+      <c r="U68" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="V68">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A53:A64"/>
     <mergeCell ref="A49:A52"/>
     <mergeCell ref="A43:A48"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A53:A68"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A22:A26"/>
@@ -20361,10 +20613,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03224E0E-0471-4EB9-BE20-7A75388FABD1}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20372,46 +20624,114 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="63">
+      <c r="B1" s="67">
         <v>1</v>
       </c>
-      <c r="C1" s="63">
+      <c r="C1" s="67">
         <v>2</v>
       </c>
-      <c r="D1" s="63">
+      <c r="D1" s="67">
         <v>3</v>
       </c>
-      <c r="E1" s="63">
+      <c r="E1" s="67">
         <v>4</v>
       </c>
-      <c r="F1" s="62">
+      <c r="F1" s="48">
         <v>5</v>
       </c>
-      <c r="G1" s="62">
+      <c r="G1" s="48">
         <v>6</v>
       </c>
-      <c r="H1" s="62">
+      <c r="H1" s="48">
         <v>7</v>
       </c>
-      <c r="I1" s="62">
+      <c r="I1" s="48">
         <v>8</v>
       </c>
-      <c r="J1" s="64">
+      <c r="J1" s="49">
         <v>9</v>
       </c>
-      <c r="K1" s="64">
+      <c r="K1" s="49">
         <v>10</v>
       </c>
-      <c r="L1" s="64">
+      <c r="L1" s="49">
         <v>11</v>
       </c>
-      <c r="M1" s="64">
+      <c r="M1" s="49">
         <v>12</v>
       </c>
+      <c r="N1" s="68">
+        <v>13</v>
+      </c>
+      <c r="O1" s="68">
+        <v>14</v>
+      </c>
+      <c r="P1" s="68">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="68">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>7694</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>68</v>
+      </c>
+      <c r="H2">
+        <v>8281</v>
+      </c>
+      <c r="I2">
+        <v>9871</v>
+      </c>
+      <c r="J2">
+        <v>81</v>
+      </c>
+      <c r="K2">
+        <v>4204</v>
+      </c>
+      <c r="L2">
+        <v>9870</v>
+      </c>
+      <c r="M2">
+        <v>9881</v>
+      </c>
+      <c r="N2">
+        <v>8584</v>
+      </c>
+      <c r="O2">
+        <v>9873</v>
+      </c>
+      <c r="P2">
+        <v>9880</v>
+      </c>
+      <c r="Q2">
+        <v>9889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G4" s="51"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q5" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20457,15 +20777,15 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
@@ -20489,18 +20809,18 @@
       <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60" t="s">
+      <c r="K2" s="65"/>
+      <c r="L2" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60" t="s">
+      <c r="M2" s="65"/>
+      <c r="N2" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="60"/>
+      <c r="O2" s="65"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
@@ -20527,18 +20847,18 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="60">
+      <c r="J3" s="65">
         <v>1.2</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60">
+      <c r="K3" s="65"/>
+      <c r="L3" s="65">
         <v>3</v>
       </c>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60">
+      <c r="M3" s="65"/>
+      <c r="N3" s="65">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="60"/>
+      <c r="O3" s="65"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
@@ -20565,18 +20885,18 @@
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="J4" s="60">
+      <c r="J4" s="65">
         <v>1.3</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60">
+      <c r="K4" s="65"/>
+      <c r="L4" s="65">
         <v>4</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60">
+      <c r="M4" s="65"/>
+      <c r="N4" s="65">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="60"/>
+      <c r="O4" s="65"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
@@ -20603,18 +20923,18 @@
       <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5" s="60">
+      <c r="J5" s="65">
         <v>2.36</v>
       </c>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60">
+      <c r="K5" s="65"/>
+      <c r="L5" s="65">
         <v>6</v>
       </c>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60">
+      <c r="M5" s="65"/>
+      <c r="N5" s="65">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="60"/>
+      <c r="O5" s="65"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -20641,18 +20961,18 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="65">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60">
+      <c r="K6" s="65"/>
+      <c r="L6" s="65">
         <v>8</v>
       </c>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60">
+      <c r="M6" s="65"/>
+      <c r="N6" s="65">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="60"/>
+      <c r="O6" s="65"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
@@ -20679,18 +20999,18 @@
       <c r="I7">
         <v>1000</v>
       </c>
-      <c r="J7" s="60">
+      <c r="J7" s="65">
         <v>3.55</v>
       </c>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60">
+      <c r="K7" s="65"/>
+      <c r="L7" s="65">
         <v>12</v>
       </c>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60">
+      <c r="M7" s="65"/>
+      <c r="N7" s="65">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="60"/>
+      <c r="O7" s="65"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
@@ -22745,12 +23065,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">

</xml_diff>

<commit_message>
modified table for evaluation of set 11
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE75DDB-6B11-4038-A964-3C99A1F5FDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6CB93A-7414-4B0F-88F5-9CD9083C5EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -776,6 +776,23 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="15"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -797,29 +814,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" xfId="15"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="16" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
@@ -14673,11 +14673,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
   <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H73" sqref="H73"/>
+      <selection pane="bottomRight" activeCell="U53" sqref="U53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14775,7 +14775,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="60" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4">
@@ -14844,7 +14844,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14911,7 +14911,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14979,7 +14979,7 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -15047,7 +15047,7 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -15116,7 +15116,7 @@
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15185,7 +15185,7 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -15251,7 +15251,7 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="66" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="5">
@@ -15322,7 +15322,7 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -15391,7 +15391,7 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="5">
         <v>3</v>
       </c>
@@ -15460,7 +15460,7 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="5">
         <v>4</v>
       </c>
@@ -15529,7 +15529,7 @@
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6">
@@ -15599,7 +15599,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="6">
         <v>2</v>
       </c>
@@ -15667,7 +15667,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -15735,7 +15735,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="6">
         <v>4</v>
       </c>
@@ -15803,7 +15803,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="6">
         <v>5</v>
       </c>
@@ -15871,7 +15871,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="6">
         <v>6</v>
       </c>
@@ -16009,7 +16009,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16">
@@ -16079,7 +16079,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="16">
         <v>2</v>
       </c>
@@ -16147,7 +16147,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="63" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="10">
@@ -16217,7 +16217,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="11">
         <v>2</v>
       </c>
@@ -16285,7 +16285,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="56"/>
+      <c r="A24" s="63"/>
       <c r="B24" s="10">
         <v>3</v>
       </c>
@@ -16353,7 +16353,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="11">
         <v>4</v>
       </c>
@@ -16421,7 +16421,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10">
         <v>5</v>
       </c>
@@ -16489,7 +16489,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="64" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="12">
@@ -16559,7 +16559,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="12">
         <v>2</v>
       </c>
@@ -16627,7 +16627,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="12">
         <v>3</v>
       </c>
@@ -16695,7 +16695,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="12">
         <v>4</v>
       </c>
@@ -16763,7 +16763,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="12">
         <v>5</v>
       </c>
@@ -16831,7 +16831,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="12">
         <v>6</v>
       </c>
@@ -16899,7 +16899,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="58" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="14">
@@ -16969,7 +16969,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="64"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -17037,7 +17037,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="64"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="14">
         <v>3</v>
       </c>
@@ -17105,7 +17105,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="64"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="14">
         <v>4</v>
       </c>
@@ -17173,7 +17173,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="64"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -17241,7 +17241,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="57" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="19">
@@ -17310,7 +17310,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="63"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="19">
         <v>2</v>
       </c>
@@ -17377,7 +17377,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="63"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="19">
         <v>3</v>
       </c>
@@ -17444,7 +17444,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="63"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="19">
         <v>4</v>
       </c>
@@ -17511,7 +17511,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="63"/>
+      <c r="A42" s="57"/>
       <c r="B42" s="19">
         <v>5</v>
       </c>
@@ -17578,7 +17578,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="62" t="s">
+      <c r="A43" s="56" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="23">
@@ -17648,7 +17648,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="62"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="23">
         <v>2</v>
       </c>
@@ -17716,7 +17716,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="62"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="23">
         <v>3</v>
       </c>
@@ -17784,7 +17784,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="62"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="23">
         <v>4</v>
       </c>
@@ -17852,7 +17852,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="62"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="23">
         <v>5</v>
       </c>
@@ -17920,7 +17920,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="62"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="23">
         <v>6</v>
       </c>
@@ -17985,7 +17985,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="61" t="s">
+      <c r="A49" s="55" t="s">
         <v>99</v>
       </c>
       <c r="B49" s="23">
@@ -18046,7 +18046,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="61"/>
+      <c r="A50" s="55"/>
       <c r="B50" s="23">
         <v>2</v>
       </c>
@@ -18101,7 +18101,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="61"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="23">
         <v>3</v>
       </c>
@@ -18156,7 +18156,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="61"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="23">
         <v>4</v>
       </c>
@@ -18211,7 +18211,7 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="60" t="s">
+      <c r="A53" s="59" t="s">
         <v>98</v>
       </c>
       <c r="B53" s="45">
@@ -18268,7 +18268,7 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="60"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="45">
         <v>2</v>
       </c>
@@ -18323,7 +18323,7 @@
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="60"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="45">
         <v>3</v>
       </c>
@@ -18378,7 +18378,7 @@
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="60"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="45">
         <v>4</v>
       </c>
@@ -18435,7 +18435,7 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="60"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="45">
         <v>5</v>
       </c>
@@ -18490,7 +18490,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="60"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="45">
         <v>6</v>
       </c>
@@ -18545,7 +18545,7 @@
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="60"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="45">
         <v>7</v>
       </c>
@@ -18600,7 +18600,7 @@
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="60"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="45">
         <v>8</v>
       </c>
@@ -18655,7 +18655,7 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="60"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="45">
         <v>9</v>
       </c>
@@ -18709,7 +18709,7 @@
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="60"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="45">
         <v>10</v>
       </c>
@@ -18763,7 +18763,7 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="60"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="45">
         <v>11</v>
       </c>
@@ -18817,7 +18817,7 @@
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="60"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="45">
         <v>12</v>
       </c>
@@ -18871,7 +18871,7 @@
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A65" s="60"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="45">
         <v>13</v>
       </c>
@@ -18925,7 +18925,7 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A66" s="60"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="45">
         <v>14</v>
       </c>
@@ -18979,7 +18979,7 @@
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A67" s="60"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="45">
         <v>15</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A68" s="60"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="45">
         <v>16</v>
       </c>
@@ -19088,17 +19088,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A53:A68"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A53:A68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20613,10 +20613,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03224E0E-0471-4EB9-BE20-7A75388FABD1}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20624,20 +20624,20 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="67">
+      <c r="B1" s="53">
         <v>1</v>
       </c>
-      <c r="C1" s="67">
+      <c r="C1" s="53">
         <v>2</v>
       </c>
-      <c r="D1" s="67">
+      <c r="D1" s="53">
         <v>3</v>
       </c>
-      <c r="E1" s="67">
+      <c r="E1" s="53">
         <v>4</v>
       </c>
       <c r="F1" s="48">
@@ -20664,73 +20664,73 @@
       <c r="M1" s="49">
         <v>12</v>
       </c>
-      <c r="N1" s="68">
+      <c r="N1" s="54">
         <v>13</v>
       </c>
-      <c r="O1" s="68">
+      <c r="O1" s="54">
         <v>14</v>
       </c>
-      <c r="P1" s="68">
+      <c r="P1" s="54">
         <v>15</v>
       </c>
-      <c r="Q1" s="68">
+      <c r="Q1" s="54">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="R2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="S2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="T2">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="U2">
         <v>7694</v>
       </c>
-      <c r="F2">
+      <c r="V2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="W2">
         <v>68</v>
       </c>
-      <c r="H2">
+      <c r="X2">
         <v>8281</v>
       </c>
-      <c r="I2">
+      <c r="Y2">
         <v>9871</v>
       </c>
-      <c r="J2">
+      <c r="Z2">
         <v>81</v>
       </c>
-      <c r="K2">
+      <c r="AA2">
         <v>4204</v>
       </c>
-      <c r="L2">
+      <c r="AB2">
         <v>9870</v>
       </c>
-      <c r="M2">
+      <c r="AC2">
         <v>9881</v>
       </c>
-      <c r="N2">
+      <c r="AD2">
         <v>8584</v>
       </c>
-      <c r="O2">
+      <c r="AE2">
         <v>9873</v>
       </c>
-      <c r="P2">
+      <c r="AF2">
         <v>9880</v>
       </c>
-      <c r="Q2">
+      <c r="AG2">
         <v>9889</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="G4" s="51"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q5" s="52"/>
     </row>
   </sheetData>
@@ -20777,15 +20777,15 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
@@ -20809,18 +20809,18 @@
       <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65" t="s">
+      <c r="K2" s="68"/>
+      <c r="L2" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65" t="s">
+      <c r="M2" s="68"/>
+      <c r="N2" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="65"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
@@ -20847,18 +20847,18 @@
       <c r="I3">
         <v>10</v>
       </c>
-      <c r="J3" s="65">
+      <c r="J3" s="68">
         <v>1.2</v>
       </c>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65">
+      <c r="K3" s="68"/>
+      <c r="L3" s="68">
         <v>3</v>
       </c>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65">
+      <c r="M3" s="68"/>
+      <c r="N3" s="68">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="65"/>
+      <c r="O3" s="68"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
@@ -20885,18 +20885,18 @@
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="J4" s="65">
+      <c r="J4" s="68">
         <v>1.3</v>
       </c>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65">
+      <c r="K4" s="68"/>
+      <c r="L4" s="68">
         <v>4</v>
       </c>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65">
+      <c r="M4" s="68"/>
+      <c r="N4" s="68">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="65"/>
+      <c r="O4" s="68"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
@@ -20923,18 +20923,18 @@
       <c r="I5">
         <v>50</v>
       </c>
-      <c r="J5" s="65">
+      <c r="J5" s="68">
         <v>2.36</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65">
+      <c r="K5" s="68"/>
+      <c r="L5" s="68">
         <v>6</v>
       </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65">
+      <c r="M5" s="68"/>
+      <c r="N5" s="68">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="65"/>
+      <c r="O5" s="68"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
@@ -20961,18 +20961,18 @@
       <c r="I6">
         <v>100</v>
       </c>
-      <c r="J6" s="65">
+      <c r="J6" s="68">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65">
+      <c r="K6" s="68"/>
+      <c r="L6" s="68">
         <v>8</v>
       </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65">
+      <c r="M6" s="68"/>
+      <c r="N6" s="68">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="65"/>
+      <c r="O6" s="68"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
@@ -20999,18 +20999,18 @@
       <c r="I7">
         <v>1000</v>
       </c>
-      <c r="J7" s="65">
+      <c r="J7" s="68">
         <v>3.55</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65">
+      <c r="K7" s="68"/>
+      <c r="L7" s="68">
         <v>12</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65">
+      <c r="M7" s="68"/>
+      <c r="N7" s="68">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="65"/>
+      <c r="O7" s="68"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
@@ -22994,6 +22994,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
@@ -23004,15 +23013,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23065,12 +23065,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">

</xml_diff>

<commit_message>
Added results from sim2 on 5k networks
</commit_message>
<xml_diff>
--- a/Data Collections/Data Collection Sim 2.xlsx
+++ b/Data Collections/Data Collection Sim 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D7E75F-0A12-4656-99E3-1C64C415E26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3560E7C-EF58-46B8-89C5-A05CA0333B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BCACAF04-D4C4-41AE-BAB0-4F6EFB70057E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planning" sheetId="3" r:id="rId1"/>
@@ -26,10 +26,10 @@
     <sheet name="Set11" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$61</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$62:$E$161</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Set4'!$E$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Set4'!$E$5:$E$54</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Set4'!$E$61</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Set4'!$E$62:$E$161</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="110">
   <si>
     <t>Evil Node Sleeping Transactions</t>
   </si>
@@ -396,7 +396,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +497,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -699,7 +705,7 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -791,21 +797,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -827,16 +825,27 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
@@ -1008,10 +1017,10 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>'Set1'!$B$103:$G$103</c:f>
+              <c:f>'Set1'!$B$103:$H$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.4701979999999999</c:v>
                 </c:pt>
@@ -1029,6 +1038,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.799436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0836990000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5928,7 +5940,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5966,7 +5978,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-BA23-47F0-8325-162A3EB2469F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -5994,7 +6006,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6032,7 +6044,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-92AE-4E86-80B1-3A198ACB5431}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Standardized </cx:v>
             </cx:txData>
           </cx:tx>
@@ -13699,16 +13711,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220981</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>27710</xdr:rowOff>
+      <xdr:rowOff>73430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>220981</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>69274</xdr:rowOff>
+      <xdr:rowOff>114994</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14688,13 +14700,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891D42F-3971-43B5-986A-C0853C8465A0}">
-  <dimension ref="A1:Y69"/>
+  <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K73" sqref="K73"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14792,7 +14804,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4">
@@ -14861,7 +14873,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -14873,7 +14885,7 @@
         <v>0.13695052585936646</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E41" si="0">LN(C3)/(C3)</f>
+        <f t="shared" ref="E3:E42" si="0">LN(C3)/(C3)</f>
         <v>0.14978661367769955</v>
       </c>
       <c r="F3" s="1">
@@ -14917,7 +14929,7 @@
         <v>100</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T60" si="1">N3</f>
+        <f t="shared" ref="T3:T61" si="1">N3</f>
         <v>10</v>
       </c>
       <c r="U3" s="44">
@@ -14928,7 +14940,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="61"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -14936,7 +14948,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D37" si="2">2*LOG(C4)/(C4-1)</f>
+        <f t="shared" ref="D4:D38" si="2">2*LOG(C4)/(C4-1)</f>
         <v>6.9345714462694649E-2</v>
       </c>
       <c r="E4" s="1">
@@ -14996,7 +15008,7 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -15064,7 +15076,7 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="61"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -15133,7 +15145,7 @@
       <c r="Y6" s="28"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="61"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -15202,93 +15214,88 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="61"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="55">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="55">
+        <f t="shared" ref="D8" si="5">2*LOG(C8)/(C8-1)</f>
+        <v>1.4798839785301135E-3</v>
+      </c>
+      <c r="E8" s="55">
+        <f>LN(C8)/(C8)</f>
+        <v>1.7034386382832477E-3</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55">
+        <v>2</v>
+      </c>
+      <c r="I8" s="55">
+        <v>100</v>
+      </c>
+      <c r="J8" s="55">
+        <v>1</v>
+      </c>
+      <c r="K8" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="55">
+        <v>10</v>
+      </c>
+      <c r="O8" s="55">
+        <v>30</v>
+      </c>
+      <c r="P8" s="55">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="S8" s="55">
+        <v>100</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8" si="6">N8</f>
+        <v>10</v>
+      </c>
+      <c r="U8" s="44">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y8" s="55"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="59"/>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>10000</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <f t="shared" si="2"/>
         <v>8.0008000800080011E-4</v>
       </c>
-      <c r="E8" s="1">
-        <f>LN(C8)/(C8)</f>
-        <v>9.210340371976184E-4</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="37">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>100</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="33">
-        <v>10</v>
-      </c>
-      <c r="O8" s="33">
-        <v>30</v>
-      </c>
-      <c r="P8" s="33">
-        <v>60</v>
-      </c>
-      <c r="Q8" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="S8" s="28">
-        <v>100</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="U8" s="44">
-        <v>0</v>
-      </c>
-      <c r="V8" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>500</v>
-      </c>
-      <c r="D9" s="1">
-        <f>2*LOG(C9)/(C9-1)</f>
-        <v>1.0817515047438954E-2</v>
-      </c>
       <c r="E9" s="1">
         <f>LN(C9)/(C9)</f>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F9" s="1">
-        <f>E9</f>
-        <v>1.2429216196844383E-2</v>
-      </c>
+        <v>9.210340371976184E-4</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="18"/>
       <c r="H9" s="37">
         <v>2</v>
@@ -15339,11 +15346,13 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
+      <c r="A10" s="64" t="s">
+        <v>19</v>
+      </c>
       <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="28">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>500</v>
       </c>
       <c r="D10" s="1">
@@ -15354,8 +15363,8 @@
         <f>LN(C10)/(C10)</f>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="F10" s="28">
-        <f t="shared" ref="F10:F48" si="5">E10</f>
+      <c r="F10" s="1">
+        <f>E10</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G10" s="18"/>
@@ -15366,7 +15375,7 @@
         <v>100</v>
       </c>
       <c r="J10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>8</v>
@@ -15407,24 +15416,24 @@
       </c>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
       <c r="B11" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="28">
         <v>500</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
+        <f>2*LOG(C11)/(C11-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f>LN(C11)/(C11)</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F11" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F11:F49" si="7">E11</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G11" s="18"/>
@@ -15435,7 +15444,7 @@
         <v>100</v>
       </c>
       <c r="J11" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>8</v>
@@ -15477,42 +15486,42 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="28">
         <v>500</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="1">
         <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F12" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="37">
         <v>2</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="1">
         <v>100</v>
       </c>
-      <c r="J12" s="22">
-        <v>20</v>
-      </c>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="1">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="N12" s="33">
@@ -15543,47 +15552,45 @@
       <c r="V12" t="s">
         <v>94</v>
       </c>
-      <c r="Y12" s="22"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="5">
+        <v>4</v>
       </c>
       <c r="C13" s="28">
         <v>500</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="22">
         <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="22">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F13" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="37">
         <v>2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="22">
         <v>100</v>
       </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="22">
+        <v>20</v>
+      </c>
+      <c r="K13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="L13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="22" t="s">
         <v>10</v>
       </c>
       <c r="N13" s="33">
@@ -15614,11 +15621,14 @@
       <c r="V13" t="s">
         <v>94</v>
       </c>
+      <c r="Y13" s="22"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="60" t="s">
+        <v>20</v>
+      </c>
       <c r="B14" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="28">
         <v>500</v>
@@ -15632,7 +15642,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F14" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G14" s="18"/>
@@ -15649,7 +15659,7 @@
         <v>8</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>10</v>
@@ -15684,9 +15694,9 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="28">
         <v>500</v>
@@ -15700,7 +15710,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F15" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G15" s="18"/>
@@ -15717,7 +15727,7 @@
         <v>8</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>10</v>
@@ -15752,9 +15762,9 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="28">
         <v>500</v>
@@ -15768,7 +15778,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F16" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G16" s="18"/>
@@ -15785,7 +15795,7 @@
         <v>8</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>10</v>
@@ -15820,9 +15830,9 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="28">
         <v>500</v>
@@ -15836,7 +15846,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F17" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G17" s="18"/>
@@ -15853,7 +15863,7 @@
         <v>8</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>10</v>
@@ -15888,9 +15898,9 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="62"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="28">
         <v>500</v>
@@ -15904,7 +15914,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F18" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G18" s="18"/>
@@ -15921,7 +15931,7 @@
         <v>8</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>10</v>
@@ -15955,12 +15965,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="60"/>
+      <c r="B19" s="6">
+        <v>6</v>
       </c>
       <c r="C19" s="28">
         <v>500</v>
@@ -15974,7 +15982,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F19" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G19" s="18"/>
@@ -15991,7 +15999,7 @@
         <v>8</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>10</v>
@@ -16025,11 +16033,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="16">
+    <row r="20" spans="1:22" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8">
         <v>1</v>
       </c>
       <c r="C20" s="28">
@@ -16044,7 +16052,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F20" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G20" s="18"/>
@@ -16096,9 +16104,11 @@
       </c>
     </row>
     <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="63" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="28">
         <v>500</v>
@@ -16112,7 +16122,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F21" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G21" s="18"/>
@@ -16163,12 +16173,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="10">
-        <v>1</v>
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63"/>
+      <c r="B22" s="16">
+        <v>2</v>
       </c>
       <c r="C22" s="28">
         <v>500</v>
@@ -16182,7 +16190,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F22" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G22" s="18"/>
@@ -16196,7 +16204,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>7</v>
@@ -16234,9 +16242,11 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="11">
-        <v>2</v>
+      <c r="A23" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
       </c>
       <c r="C23" s="28">
         <v>500</v>
@@ -16250,7 +16260,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F23" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G23" s="18"/>
@@ -16264,7 +16274,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>7</v>
@@ -16302,9 +16312,9 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
-      <c r="B24" s="10">
-        <v>3</v>
+      <c r="A24" s="61"/>
+      <c r="B24" s="11">
+        <v>2</v>
       </c>
       <c r="C24" s="28">
         <v>500</v>
@@ -16318,7 +16328,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F24" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G24" s="18"/>
@@ -16332,7 +16342,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>7</v>
@@ -16370,9 +16380,9 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="11">
-        <v>4</v>
+      <c r="A25" s="61"/>
+      <c r="B25" s="10">
+        <v>3</v>
       </c>
       <c r="C25" s="28">
         <v>500</v>
@@ -16386,7 +16396,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F25" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G25" s="18"/>
@@ -16400,7 +16410,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>7</v>
@@ -16438,9 +16448,9 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="10">
-        <v>5</v>
+      <c r="A26" s="61"/>
+      <c r="B26" s="11">
+        <v>4</v>
       </c>
       <c r="C26" s="28">
         <v>500</v>
@@ -16454,7 +16464,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F26" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G26" s="18"/>
@@ -16468,7 +16478,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>7</v>
@@ -16480,10 +16490,10 @@
         <v>10</v>
       </c>
       <c r="O26" s="33">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="P26" s="33">
-        <v>600</v>
+        <v>60</v>
       </c>
       <c r="Q26" s="33" t="s">
         <v>83</v>
@@ -16506,17 +16516,15 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="12">
-        <v>1</v>
+      <c r="A27" s="61"/>
+      <c r="B27" s="10">
+        <v>5</v>
       </c>
       <c r="C27" s="28">
         <v>500</v>
       </c>
       <c r="D27" s="1">
-        <f>2*LOG(C27)/(C27-1)</f>
+        <f t="shared" si="2"/>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E27" s="1">
@@ -16524,12 +16532,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F27" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G27" s="18"/>
-      <c r="H27" s="1">
-        <v>1</v>
+      <c r="H27" s="37">
+        <v>2</v>
       </c>
       <c r="I27" s="1">
         <v>100</v>
@@ -16538,7 +16546,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>7</v>
@@ -16550,10 +16558,10 @@
         <v>10</v>
       </c>
       <c r="O27" s="33">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="P27" s="33">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="Q27" s="33" t="s">
         <v>83</v>
@@ -16576,9 +16584,11 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="64"/>
+      <c r="A28" s="62" t="s">
+        <v>48</v>
+      </c>
       <c r="B28" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="28">
         <v>500</v>
@@ -16592,12 +16602,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F28" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" s="1">
         <v>100</v>
@@ -16644,15 +16654,15 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="28">
         <v>500</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="2"/>
+        <f>2*LOG(C29)/(C29-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E29" s="1">
@@ -16660,12 +16670,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F29" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1">
         <v>100</v>
@@ -16712,9 +16722,9 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="64"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="28">
         <v>500</v>
@@ -16728,12 +16738,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F30" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1">
         <v>100</v>
@@ -16780,9 +16790,9 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="28">
         <v>500</v>
@@ -16796,12 +16806,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F31" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I31" s="1">
         <v>100</v>
@@ -16848,9 +16858,9 @@
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="64"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="28">
         <v>500</v>
@@ -16864,12 +16874,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F32" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I32" s="1">
         <v>100</v>
@@ -16916,11 +16926,9 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A33" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="14">
-        <v>1</v>
+      <c r="A33" s="62"/>
+      <c r="B33" s="12">
+        <v>6</v>
       </c>
       <c r="C33" s="28">
         <v>500</v>
@@ -16934,12 +16942,12 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F33" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="1">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="I33" s="1">
         <v>100</v>
@@ -16954,7 +16962,7 @@
         <v>7</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="N33" s="33">
         <v>10</v>
@@ -16986,9 +16994,11 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
+      <c r="A34" s="68" t="s">
+        <v>49</v>
+      </c>
       <c r="B34" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="28">
         <v>500</v>
@@ -17002,11 +17012,11 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F34" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G34" s="18"/>
-      <c r="H34" s="37">
+      <c r="H34" s="1">
         <v>2</v>
       </c>
       <c r="I34" s="1">
@@ -17022,7 +17032,7 @@
         <v>7</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N34" s="33">
         <v>10</v>
@@ -17054,9 +17064,9 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="28">
         <v>500</v>
@@ -17070,7 +17080,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F35" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G35" s="18"/>
@@ -17090,7 +17100,7 @@
         <v>7</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N35" s="33">
         <v>10</v>
@@ -17122,9 +17132,9 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A36" s="58"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="28">
         <v>500</v>
@@ -17138,7 +17148,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F36" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G36" s="18"/>
@@ -17158,7 +17168,7 @@
         <v>7</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N36" s="33">
         <v>10</v>
@@ -17190,9 +17200,9 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="28">
         <v>500</v>
@@ -17206,7 +17216,7 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F37" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G37" s="18"/>
@@ -17226,7 +17236,7 @@
         <v>7</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N37" s="33">
         <v>10</v>
@@ -17258,44 +17268,43 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="19">
-        <v>1</v>
+      <c r="A38" s="68"/>
+      <c r="B38" s="14">
+        <v>5</v>
       </c>
       <c r="C38" s="28">
         <v>500</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="18">
+      <c r="D38" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E38" s="1">
         <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F38" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G38" s="18">
-        <v>1</v>
-      </c>
+      <c r="G38" s="18"/>
       <c r="H38" s="37">
         <v>2</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="1">
         <v>100</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="1">
         <v>1</v>
       </c>
-      <c r="K38" s="18" t="s">
+      <c r="K38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="18" t="s">
+      <c r="L38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="24" t="s">
-        <v>10</v>
+      <c r="M38" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="N38" s="33">
         <v>10</v>
@@ -17327,9 +17336,11 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A39" s="57"/>
+      <c r="A39" s="67" t="s">
+        <v>80</v>
+      </c>
       <c r="B39" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="28">
         <v>500</v>
@@ -17340,11 +17351,11 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F39" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G39" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="37">
         <v>2</v>
@@ -17394,9 +17405,9 @@
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="57"/>
+      <c r="A40" s="67"/>
       <c r="B40" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="28">
         <v>500</v>
@@ -17407,11 +17418,11 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F40" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G40" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H40" s="37">
         <v>2</v>
@@ -17461,9 +17472,9 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="57"/>
+      <c r="A41" s="67"/>
       <c r="B41" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="28">
         <v>500</v>
@@ -17474,11 +17485,11 @@
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F41" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G41" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H41" s="37">
         <v>2</v>
@@ -17528,24 +17539,24 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="57"/>
+      <c r="A42" s="67"/>
       <c r="B42" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="28">
         <v>500</v>
       </c>
-      <c r="D42" s="18"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="18">
-        <f t="shared" ref="E42:E48" si="6">LN(C42)/(C42)</f>
+        <f t="shared" si="0"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F42" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G42" s="18">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H42" s="37">
         <v>2</v>
@@ -17594,63 +17605,60 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="23">
-        <v>1</v>
-      </c>
-      <c r="C43" s="37">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A43" s="67"/>
+      <c r="B43" s="19">
+        <v>5</v>
+      </c>
+      <c r="C43" s="28">
         <v>500</v>
       </c>
-      <c r="D43" s="20">
-        <f>2*LOG(C43)/(C43-1)</f>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E43" s="20">
-        <f t="shared" si="6"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18">
+        <f t="shared" ref="E43:E49" si="8">LN(C43)/(C43)</f>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F43" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="G43" s="20"/>
+      <c r="G43" s="18">
+        <v>100</v>
+      </c>
       <c r="H43" s="37">
         <v>2</v>
       </c>
-      <c r="I43" s="37">
+      <c r="I43" s="18">
         <v>100</v>
       </c>
-      <c r="J43" s="37">
+      <c r="J43" s="18">
         <v>1</v>
       </c>
-      <c r="K43" s="37" t="s">
+      <c r="K43" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L43" s="37" t="s">
+      <c r="L43" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="37" t="s">
+      <c r="M43" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N43" s="37">
+      <c r="N43" s="33">
         <v>10</v>
       </c>
-      <c r="O43" s="37">
+      <c r="O43" s="33">
         <v>30</v>
       </c>
-      <c r="P43" s="37">
+      <c r="P43" s="33">
         <v>60</v>
       </c>
-      <c r="Q43" s="37" t="s">
+      <c r="Q43" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="R43" s="37" t="s">
+      <c r="R43" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="S43" s="37">
+      <c r="S43" s="28">
         <v>100</v>
       </c>
       <c r="T43">
@@ -17664,10 +17672,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="56"/>
+    <row r="44" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="66" t="s">
+        <v>81</v>
+      </c>
       <c r="B44" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="37">
         <v>500</v>
@@ -17677,11 +17687,11 @@
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E44" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F44" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G44" s="20"/>
@@ -17733,23 +17743,23 @@
       </c>
     </row>
     <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="56"/>
+      <c r="A45" s="66"/>
       <c r="B45" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="37">
         <v>500</v>
       </c>
       <c r="D45" s="20">
-        <f t="shared" ref="D45:D47" si="7">2*LOG(C45)/(C45-1)</f>
+        <f>2*LOG(C45)/(C45-1)</f>
         <v>1.0817515047438954E-2</v>
       </c>
       <c r="E45" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F45" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G45" s="20"/>
@@ -17801,23 +17811,23 @@
       </c>
     </row>
     <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="37">
         <v>500</v>
       </c>
       <c r="D46" s="20">
+        <f t="shared" ref="D46:D48" si="9">2*LOG(C46)/(C46-1)</f>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E46" s="20">
+        <f t="shared" si="8"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F46" s="28">
         <f t="shared" si="7"/>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E46" s="20">
-        <f t="shared" si="6"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="F46" s="28">
-        <f t="shared" si="5"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G46" s="20"/>
@@ -17869,26 +17879,26 @@
       </c>
     </row>
     <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="56"/>
+      <c r="A47" s="66"/>
       <c r="B47" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="37">
         <v>500</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="20">
+        <f t="shared" si="9"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
+      <c r="E47" s="20">
+        <f t="shared" si="8"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F47" s="28">
         <f t="shared" si="7"/>
-        <v>1.0817515047438954E-2</v>
-      </c>
-      <c r="E47" s="22">
-        <f t="shared" si="6"/>
         <v>1.2429216196844383E-2</v>
       </c>
-      <c r="F47" s="28">
-        <f t="shared" si="5"/>
-        <v>1.2429216196844383E-2</v>
-      </c>
-      <c r="G47" s="22"/>
+      <c r="G47" s="20"/>
       <c r="H47" s="37">
         <v>2</v>
       </c>
@@ -17937,20 +17947,23 @@
       </c>
     </row>
     <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="56"/>
+      <c r="A48" s="66"/>
       <c r="B48" s="23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="37">
         <v>500</v>
       </c>
-      <c r="D48" s="22"/>
+      <c r="D48" s="22">
+        <f t="shared" si="9"/>
+        <v>1.0817515047438954E-2</v>
+      </c>
       <c r="E48" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="F48" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.2429216196844383E-2</v>
       </c>
       <c r="G48" s="22"/>
@@ -18001,20 +18014,24 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="55" t="s">
-        <v>99</v>
-      </c>
+    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="66"/>
       <c r="B49" s="23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C49" s="37">
         <v>500</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="18"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22">
+        <f t="shared" si="8"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="F49" s="28">
+        <f t="shared" si="7"/>
+        <v>1.2429216196844383E-2</v>
+      </c>
+      <c r="G49" s="22"/>
       <c r="H49" s="37">
         <v>2</v>
       </c>
@@ -18034,7 +18051,7 @@
         <v>10</v>
       </c>
       <c r="N49" s="37">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O49" s="37">
         <v>30</v>
@@ -18053,7 +18070,7 @@
       </c>
       <c r="T49">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U49" s="44">
         <v>0</v>
@@ -18063,13 +18080,19 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="55"/>
+      <c r="A50" s="65" t="s">
+        <v>99</v>
+      </c>
       <c r="B50" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" s="37">
         <v>500</v>
       </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="37">
         <v>2</v>
       </c>
@@ -18089,7 +18112,7 @@
         <v>10</v>
       </c>
       <c r="N50" s="37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="O50" s="37">
         <v>30</v>
@@ -18108,7 +18131,7 @@
       </c>
       <c r="T50">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="U50" s="44">
         <v>0</v>
@@ -18118,9 +18141,9 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="55"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="37">
         <v>500</v>
@@ -18144,7 +18167,7 @@
         <v>10</v>
       </c>
       <c r="N51" s="37">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="O51" s="37">
         <v>30</v>
@@ -18163,7 +18186,7 @@
       </c>
       <c r="T51">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="U51" s="44">
         <v>0</v>
@@ -18173,9 +18196,9 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="55"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="37">
         <v>500</v>
@@ -18198,8 +18221,8 @@
       <c r="M52" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="N52" s="37" t="s">
-        <v>90</v>
+      <c r="N52" s="37">
+        <v>100</v>
       </c>
       <c r="O52" s="37">
         <v>30</v>
@@ -18216,78 +18239,78 @@
       <c r="S52" s="37">
         <v>100</v>
       </c>
-      <c r="T52" s="47" t="str">
+      <c r="T52">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="U52" s="44">
+        <v>0</v>
+      </c>
+      <c r="V52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A53" s="65"/>
+      <c r="B53" s="23">
+        <v>4</v>
+      </c>
+      <c r="C53" s="37">
+        <v>500</v>
+      </c>
+      <c r="H53" s="37">
+        <v>2</v>
+      </c>
+      <c r="I53" s="37">
+        <v>100</v>
+      </c>
+      <c r="J53" s="37">
+        <v>1</v>
+      </c>
+      <c r="K53" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="L53" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N53" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="O53" s="37">
+        <v>30</v>
+      </c>
+      <c r="P53" s="37">
+        <v>60</v>
+      </c>
+      <c r="Q53" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="R53" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="S53" s="37">
+        <v>100</v>
+      </c>
+      <c r="T53" s="47" t="str">
         <f t="shared" si="1"/>
         <v>Max</v>
       </c>
-      <c r="U52" s="44">
+      <c r="U53" s="44">
         <v>0</v>
       </c>
-      <c r="V52" t="s">
+      <c r="V53" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="59" t="s">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A54" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="45">
+      <c r="B54" s="45">
         <v>1</v>
-      </c>
-      <c r="C53" s="43">
-        <v>500</v>
-      </c>
-      <c r="H53" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="I53" s="43">
-        <v>100</v>
-      </c>
-      <c r="J53" s="43">
-        <v>0</v>
-      </c>
-      <c r="K53" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="L53" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="M53" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N53" s="43">
-        <v>30</v>
-      </c>
-      <c r="O53" s="43">
-        <v>30</v>
-      </c>
-      <c r="P53" s="43">
-        <v>60</v>
-      </c>
-      <c r="Q53" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="R53" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="S53" s="43">
-        <v>100</v>
-      </c>
-      <c r="T53">
-        <f>N53*0.3</f>
-        <v>9</v>
-      </c>
-      <c r="U53" s="44">
-        <v>0.05</v>
-      </c>
-      <c r="V53">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="59"/>
-      <c r="B54" s="45">
-        <v>2</v>
       </c>
       <c r="C54" s="43">
         <v>500</v>
@@ -18329,8 +18352,8 @@
         <v>100</v>
       </c>
       <c r="T54">
-        <f>N54*0.5</f>
-        <v>15</v>
+        <f>N54*0.3</f>
+        <v>9</v>
       </c>
       <c r="U54" s="44">
         <v>0.05</v>
@@ -18340,9 +18363,9 @@
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="59"/>
+      <c r="A55" s="69"/>
       <c r="B55" s="45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="43">
         <v>500</v>
@@ -18384,8 +18407,8 @@
         <v>100</v>
       </c>
       <c r="T55">
-        <f>N55*0.8</f>
-        <v>24</v>
+        <f>N55*0.5</f>
+        <v>15</v>
       </c>
       <c r="U55" s="44">
         <v>0.05</v>
@@ -18395,15 +18418,13 @@
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="59"/>
+      <c r="A56" s="69"/>
       <c r="B56" s="45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" s="43">
         <v>500</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
       <c r="H56" s="46" t="s">
         <v>96</v>
       </c>
@@ -18441,75 +18462,77 @@
         <v>100</v>
       </c>
       <c r="T56">
+        <f>N56*0.8</f>
+        <v>24</v>
+      </c>
+      <c r="U56" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="V56">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A57" s="69"/>
+      <c r="B57" s="45">
+        <v>4</v>
+      </c>
+      <c r="C57" s="43">
+        <v>500</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I57" s="43">
+        <v>100</v>
+      </c>
+      <c r="J57" s="43">
+        <v>0</v>
+      </c>
+      <c r="K57" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L57" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" s="43">
+        <v>30</v>
+      </c>
+      <c r="O57" s="43">
+        <v>30</v>
+      </c>
+      <c r="P57" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q57" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R57" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S57" s="43">
+        <v>100</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="U56" s="44">
+      <c r="U57" s="44">
         <v>0.05</v>
-      </c>
-      <c r="V56">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="59"/>
-      <c r="B57" s="45">
-        <v>5</v>
-      </c>
-      <c r="C57" s="43">
-        <v>500</v>
-      </c>
-      <c r="H57" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="I57" s="43">
-        <v>100</v>
-      </c>
-      <c r="J57" s="43">
-        <v>0</v>
-      </c>
-      <c r="K57" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="L57" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="M57" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N57" s="43">
-        <v>30</v>
-      </c>
-      <c r="O57" s="43">
-        <v>30</v>
-      </c>
-      <c r="P57" s="43">
-        <v>60</v>
-      </c>
-      <c r="Q57" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="R57" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="S57" s="43">
-        <v>100</v>
-      </c>
-      <c r="T57">
-        <f>N57*0.3</f>
-        <v>9</v>
-      </c>
-      <c r="U57" s="44">
-        <v>0.3</v>
       </c>
       <c r="V57">
         <v>10000</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="59"/>
+      <c r="A58" s="69"/>
       <c r="B58" s="45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" s="43">
         <v>500</v>
@@ -18551,8 +18574,8 @@
         <v>100</v>
       </c>
       <c r="T58">
-        <f>N58*0.5</f>
-        <v>15</v>
+        <f>N58*0.3</f>
+        <v>9</v>
       </c>
       <c r="U58" s="44">
         <v>0.3</v>
@@ -18562,9 +18585,9 @@
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="59"/>
+      <c r="A59" s="69"/>
       <c r="B59" s="45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" s="43">
         <v>500</v>
@@ -18606,8 +18629,8 @@
         <v>100</v>
       </c>
       <c r="T59">
-        <f>N59*0.8</f>
-        <v>24</v>
+        <f>N59*0.5</f>
+        <v>15</v>
       </c>
       <c r="U59" s="44">
         <v>0.3</v>
@@ -18617,9 +18640,9 @@
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="59"/>
+      <c r="A60" s="69"/>
       <c r="B60" s="45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" s="43">
         <v>500</v>
@@ -18661,74 +18684,75 @@
         <v>100</v>
       </c>
       <c r="T60">
+        <f>N60*0.8</f>
+        <v>24</v>
+      </c>
+      <c r="U60" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="V60">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A61" s="69"/>
+      <c r="B61" s="45">
+        <v>8</v>
+      </c>
+      <c r="C61" s="43">
+        <v>500</v>
+      </c>
+      <c r="H61" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" s="43">
+        <v>100</v>
+      </c>
+      <c r="J61" s="43">
+        <v>0</v>
+      </c>
+      <c r="K61" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L61" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M61" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="N61" s="43">
+        <v>30</v>
+      </c>
+      <c r="O61" s="43">
+        <v>30</v>
+      </c>
+      <c r="P61" s="43">
+        <v>60</v>
+      </c>
+      <c r="Q61" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="R61" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="S61" s="43">
+        <v>100</v>
+      </c>
+      <c r="T61">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="U60" s="44">
+      <c r="U61" s="44">
         <v>0.3</v>
-      </c>
-      <c r="V60">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="59"/>
-      <c r="B61" s="45">
-        <v>9</v>
-      </c>
-      <c r="C61" s="43">
-        <v>500</v>
-      </c>
-      <c r="H61" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="I61" s="43">
-        <v>100</v>
-      </c>
-      <c r="J61" s="43">
-        <v>0</v>
-      </c>
-      <c r="K61" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="L61" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="M61" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="N61" s="43">
-        <v>30</v>
-      </c>
-      <c r="O61" s="43">
-        <v>30</v>
-      </c>
-      <c r="P61" s="43">
-        <v>60</v>
-      </c>
-      <c r="Q61" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="R61" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="S61" s="43">
-        <v>100</v>
-      </c>
-      <c r="T61">
-        <v>9</v>
-      </c>
-      <c r="U61" s="44">
-        <v>0.5</v>
       </c>
       <c r="V61">
         <v>10000</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="59"/>
+      <c r="A62" s="69"/>
       <c r="B62" s="45">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62" s="43">
         <v>500</v>
@@ -18770,7 +18794,7 @@
         <v>100</v>
       </c>
       <c r="T62">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="U62" s="44">
         <v>0.5</v>
@@ -18780,9 +18804,9 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="59"/>
+      <c r="A63" s="69"/>
       <c r="B63" s="45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C63" s="43">
         <v>500</v>
@@ -18824,7 +18848,7 @@
         <v>100</v>
       </c>
       <c r="T63">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U63" s="44">
         <v>0.5</v>
@@ -18834,9 +18858,9 @@
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="59"/>
+      <c r="A64" s="69"/>
       <c r="B64" s="45">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64" s="43">
         <v>500</v>
@@ -18878,7 +18902,7 @@
         <v>100</v>
       </c>
       <c r="T64">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U64" s="44">
         <v>0.5</v>
@@ -18888,63 +18912,63 @@
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A65" s="59"/>
+      <c r="A65" s="69"/>
       <c r="B65" s="45">
-        <v>13</v>
-      </c>
-      <c r="C65" s="50">
+        <v>12</v>
+      </c>
+      <c r="C65" s="43">
         <v>500</v>
       </c>
       <c r="H65" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="I65" s="50">
+      <c r="I65" s="43">
         <v>100</v>
       </c>
-      <c r="J65" s="50">
+      <c r="J65" s="43">
         <v>0</v>
       </c>
-      <c r="K65" s="50" t="s">
+      <c r="K65" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="L65" s="50" t="s">
+      <c r="L65" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="M65" s="50" t="s">
+      <c r="M65" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="N65" s="50">
+      <c r="N65" s="43">
         <v>30</v>
       </c>
-      <c r="O65" s="50">
+      <c r="O65" s="43">
         <v>30</v>
       </c>
-      <c r="P65" s="50">
+      <c r="P65" s="43">
         <v>60</v>
       </c>
-      <c r="Q65" s="50" t="s">
+      <c r="Q65" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="R65" s="50" t="s">
+      <c r="R65" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="S65" s="50">
+      <c r="S65" s="43">
         <v>100</v>
       </c>
       <c r="T65">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="U65" s="44">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="V65">
         <v>10000</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A66" s="59"/>
+      <c r="A66" s="69"/>
       <c r="B66" s="45">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66" s="50">
         <v>500</v>
@@ -18986,7 +19010,7 @@
         <v>100</v>
       </c>
       <c r="T66">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="U66" s="44">
         <v>0.8</v>
@@ -18996,9 +19020,9 @@
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A67" s="59"/>
+      <c r="A67" s="69"/>
       <c r="B67" s="45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C67" s="50">
         <v>500</v>
@@ -19040,7 +19064,7 @@
         <v>100</v>
       </c>
       <c r="T67">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U67" s="44">
         <v>0.8</v>
@@ -19050,9 +19074,9 @@
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A68" s="59"/>
+      <c r="A68" s="69"/>
       <c r="B68" s="45">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C68" s="50">
         <v>500</v>
@@ -19094,7 +19118,7 @@
         <v>100</v>
       </c>
       <c r="T68">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U68" s="44">
         <v>0.8</v>
@@ -19104,74 +19128,128 @@
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A69" s="69" t="s">
+      <c r="A69" s="69"/>
+      <c r="B69" s="45">
+        <v>16</v>
+      </c>
+      <c r="C69" s="50">
+        <v>500</v>
+      </c>
+      <c r="H69" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I69" s="50">
+        <v>100</v>
+      </c>
+      <c r="J69" s="50">
+        <v>0</v>
+      </c>
+      <c r="K69" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="L69" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M69" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="N69" s="50">
+        <v>30</v>
+      </c>
+      <c r="O69" s="50">
+        <v>30</v>
+      </c>
+      <c r="P69" s="50">
+        <v>60</v>
+      </c>
+      <c r="Q69" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="R69" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="S69" s="50">
+        <v>100</v>
+      </c>
+      <c r="T69">
+        <v>30</v>
+      </c>
+      <c r="U69" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="V69">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A70" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B69" s="70">
+      <c r="B70" s="57">
         <v>1</v>
       </c>
-      <c r="C69" s="54">
+      <c r="C70" s="54">
         <v>999</v>
       </c>
-      <c r="H69" s="54">
+      <c r="H70" s="54">
         <v>2</v>
       </c>
-      <c r="I69" s="54">
+      <c r="I70" s="54">
         <v>100</v>
       </c>
-      <c r="J69" s="54">
+      <c r="J70" s="54">
         <v>1</v>
       </c>
-      <c r="K69" s="54" t="s">
+      <c r="K70" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L69" s="54" t="s">
+      <c r="L70" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="M69" s="54" t="s">
+      <c r="M70" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="N69" s="54">
+      <c r="N70" s="54">
         <v>10</v>
       </c>
-      <c r="O69" s="54">
+      <c r="O70" s="54">
         <v>30</v>
       </c>
-      <c r="P69" s="54">
+      <c r="P70" s="54">
         <v>60</v>
       </c>
-      <c r="Q69" s="54" t="s">
+      <c r="Q70" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="R69" s="54" t="s">
+      <c r="R70" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="S69" s="54" t="s">
+      <c r="S70" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="T69">
+      <c r="T70">
         <v>10</v>
       </c>
-      <c r="U69" s="44">
+      <c r="U70" s="44">
         <v>0</v>
       </c>
-      <c r="V69" s="54" t="s">
+      <c r="V70" s="54" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A53:A68"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A54:A69"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21897,22 +21975,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF874DAA-691A-4835-ACA3-DB30922CFD6B}">
-  <dimension ref="A1:O107"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -21934,17 +22012,20 @@
       <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="H1" s="5">
+        <v>7</v>
+      </c>
+      <c r="J1" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="32">
         <v>1.5297051661450001</v>
       </c>
@@ -21963,23 +22044,26 @@
       <c r="G2" s="32">
         <v>2.87647700605</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="32">
+        <v>2.9049386641370001</v>
+      </c>
+      <c r="J2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="K2" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="70"/>
+      <c r="M2" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68" t="s">
+      <c r="N2" s="70"/>
+      <c r="O2" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="68"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="70"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="32">
         <v>1.7263440361110001</v>
       </c>
@@ -21998,26 +22082,29 @@
       <c r="G3" s="32">
         <v>2.8156623548819999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="32">
+        <v>3.0801002926719998</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3" s="68">
+      <c r="K3" s="70">
         <v>1.2</v>
       </c>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68">
+      <c r="L3" s="70"/>
+      <c r="M3" s="70">
         <v>3</v>
       </c>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68">
+      <c r="N3" s="70"/>
+      <c r="O3" s="70">
         <v>1.7929999999999999</v>
       </c>
-      <c r="O3" s="68"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="70"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" s="32">
         <v>1.848763423699</v>
       </c>
@@ -22036,26 +22123,29 @@
       <c r="G4" s="32">
         <v>2.5739380637979998</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="32">
+        <v>3.2907534423359999</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>20</v>
       </c>
-      <c r="J4" s="68">
+      <c r="K4" s="70">
         <v>1.3</v>
       </c>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68">
+      <c r="L4" s="70"/>
+      <c r="M4" s="70">
         <v>4</v>
       </c>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68">
+      <c r="N4" s="70"/>
+      <c r="O4" s="70">
         <v>1.8839999999999999</v>
       </c>
-      <c r="O4" s="68"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="70"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="32">
         <v>1.263641598302</v>
       </c>
@@ -22074,26 +22164,29 @@
       <c r="G5" s="32">
         <v>2.9062297882969998</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="32">
+        <v>3.1295994845139998</v>
+      </c>
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>50</v>
       </c>
-      <c r="J5" s="68">
+      <c r="K5" s="70">
         <v>2.36</v>
       </c>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68">
+      <c r="L5" s="70"/>
+      <c r="M5" s="70">
         <v>6</v>
       </c>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68">
+      <c r="N5" s="70"/>
+      <c r="O5" s="70">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O5" s="68"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="70"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="32">
         <v>1.525047846398</v>
       </c>
@@ -22112,26 +22205,29 @@
       <c r="G6" s="32">
         <v>2.769283006452</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="32">
+        <v>2.755269658844</v>
+      </c>
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>100</v>
       </c>
-      <c r="J6" s="68">
+      <c r="K6" s="70">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68">
+      <c r="L6" s="70"/>
+      <c r="M6" s="70">
         <v>8</v>
       </c>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68">
+      <c r="N6" s="70"/>
+      <c r="O6" s="70">
         <v>2.8820000000000001</v>
       </c>
-      <c r="O6" s="68"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="70"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="32">
         <v>1.203207808613</v>
       </c>
@@ -22150,26 +22246,29 @@
       <c r="G7" s="32">
         <v>2.5067989393399999</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="32">
+        <v>3.0779613219309998</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1000</v>
       </c>
-      <c r="J7" s="68">
+      <c r="K7" s="70">
         <v>3.55</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68">
+      <c r="L7" s="70"/>
+      <c r="M7" s="70">
         <v>12</v>
       </c>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68">
+      <c r="N7" s="70"/>
+      <c r="O7" s="70">
         <v>4.1079999999999997</v>
       </c>
-      <c r="O7" s="68"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="70"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" s="32">
         <v>1.8491733109640001</v>
       </c>
@@ -22188,8 +22287,11 @@
       <c r="G8" s="32">
         <v>2.9432894679369999</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H8" s="32">
+        <v>3.2087413870649999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="32">
         <v>1.2352078257120001</v>
       </c>
@@ -22208,8 +22310,11 @@
       <c r="G9" s="32">
         <v>2.9412920528950002</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H9" s="32">
+        <v>3.2341443740370002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="32">
         <v>1.7492208336870001</v>
       </c>
@@ -22228,8 +22333,11 @@
       <c r="G10" s="32">
         <v>2.9892566574670001</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H10" s="32">
+        <v>2.830258955928</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="32">
         <v>0.93183882744000002</v>
       </c>
@@ -22248,8 +22356,11 @@
       <c r="G11" s="32">
         <v>2.9145506056219999</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H11" s="32">
+        <v>3.1855665279899998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="32">
         <v>1.7363918421390001</v>
       </c>
@@ -22268,8 +22379,11 @@
       <c r="G12" s="32">
         <v>2.5904461169939998</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H12" s="32">
+        <v>3.2233531347870001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="32">
         <v>0.78330766388299999</v>
       </c>
@@ -22288,8 +22402,9 @@
       <c r="G13" s="32">
         <v>2.6899602528119999</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="32">
         <v>1.9209648898</v>
       </c>
@@ -22309,7 +22424,7 @@
         <v>2.8335436398359999</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="32">
         <v>1.2505701174949999</v>
       </c>
@@ -22329,7 +22444,7 @@
         <v>2.7660415201580002</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="32">
         <v>1.8069447503960001</v>
       </c>
@@ -22349,7 +22464,7 @@
         <v>2.6784192103960001</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="32">
         <v>1.2231586629860001</v>
       </c>
@@ -22369,7 +22484,7 @@
         <v>2.8691296390069998</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="32">
         <v>0.96727112336099996</v>
       </c>
@@ -22389,7 +22504,7 @@
         <v>2.8337924672089998</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="32">
         <v>1.7803714215749999</v>
       </c>
@@ -22408,8 +22523,9 @@
       <c r="G19" s="32">
         <v>2.9313078602510001</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="32">
         <v>1.267253996465</v>
       </c>
@@ -22428,8 +22544,9 @@
       <c r="G20" s="32">
         <v>2.6295201187880002</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="32">
         <v>1.5989062476310001</v>
       </c>
@@ -22448,8 +22565,9 @@
       <c r="G21" s="32">
         <v>2.482674349591</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="32">
         <v>1.6682997899859999</v>
       </c>
@@ -22468,8 +22586,9 @@
       <c r="G22" s="32">
         <v>3.0603539795939998</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="32">
         <v>1.7739574388670001</v>
       </c>
@@ -22488,8 +22607,9 @@
       <c r="G23" s="32">
         <v>2.7439563884129998</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="32">
         <v>1.189906411837</v>
       </c>
@@ -22508,8 +22628,9 @@
       <c r="G24" s="32">
         <v>2.6534886595530001</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="32"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="32">
         <v>1.60832598965</v>
       </c>
@@ -22528,8 +22649,9 @@
       <c r="G25" s="32">
         <v>2.8607121904569999</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="32">
         <v>1.585718533955</v>
       </c>
@@ -22548,8 +22670,9 @@
       <c r="G26" s="32">
         <v>2.628646721265</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="32">
         <v>1.383405570766</v>
       </c>
@@ -22568,8 +22691,9 @@
       <c r="G27" s="32">
         <v>2.698899324184</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="32"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="32">
         <v>0.98602623067399997</v>
       </c>
@@ -22588,8 +22712,9 @@
       <c r="G28" s="32">
         <v>2.969797810772</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="32">
         <v>1.3230288092039999</v>
       </c>
@@ -22608,8 +22733,9 @@
       <c r="G29" s="32">
         <v>2.5078288808729998</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="32"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="32">
         <v>1.3109761317990001</v>
       </c>
@@ -22628,8 +22754,9 @@
       <c r="G30" s="32">
         <v>2.9515851150530001</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="32"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="32">
         <v>1.551386970474</v>
       </c>
@@ -22648,8 +22775,9 @@
       <c r="G31" s="32">
         <v>3.0843254590929998</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="32"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="32">
         <v>1.339392561778</v>
       </c>
@@ -22668,8 +22796,9 @@
       <c r="G32" s="32">
         <v>3.127952823322</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="32">
         <v>1.869192395512</v>
       </c>
@@ -22688,8 +22817,9 @@
       <c r="G33" s="32">
         <v>2.9518661672239999</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="32">
         <v>1.808273226102</v>
       </c>
@@ -22708,8 +22838,9 @@
       <c r="G34" s="32">
         <v>2.8674760344900001</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="32"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="32">
         <v>1.5084261852109999</v>
       </c>
@@ -22728,8 +22859,9 @@
       <c r="G35" s="32">
         <v>2.8957382355550001</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="32">
         <v>1.3966294131570001</v>
       </c>
@@ -22748,8 +22880,9 @@
       <c r="G36" s="32">
         <v>2.4785807563660001</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="32"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="32">
         <v>1.0862525709299999</v>
       </c>
@@ -22768,8 +22901,9 @@
       <c r="G37" s="32">
         <v>2.9755182179149999</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="32"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="32">
         <v>1.339891590218</v>
       </c>
@@ -22788,8 +22922,9 @@
       <c r="G38" s="32">
         <v>2.9899073371720002</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="32"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="32">
         <v>1.6101712025829999</v>
       </c>
@@ -22808,8 +22943,9 @@
       <c r="G39" s="32">
         <v>2.7008305612410002</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="32"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="32">
         <v>1.9105397259350001</v>
       </c>
@@ -22828,8 +22964,9 @@
       <c r="G40" s="32">
         <v>2.8862471755789998</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="32"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="32">
         <v>1.7791316506579999</v>
       </c>
@@ -22848,8 +22985,9 @@
       <c r="G41" s="32">
         <v>2.8898465802620001</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="32"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" s="32">
         <v>1.3436290443409999</v>
       </c>
@@ -22868,8 +23006,9 @@
       <c r="G42" s="32">
         <v>2.8586840309000001</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="32"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="32">
         <v>1.27172572956</v>
       </c>
@@ -22888,8 +23027,9 @@
       <c r="G43" s="32">
         <v>2.7142832408999999</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="32"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="32">
         <v>1.863529605124</v>
       </c>
@@ -22908,8 +23048,9 @@
       <c r="G44" s="32">
         <v>2.8841814289990002</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="32"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="32">
         <v>1.4029948615929999</v>
       </c>
@@ -22928,8 +23069,9 @@
       <c r="G45" s="32">
         <v>3.0197270998730001</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H45" s="32"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="32">
         <v>1.0442943130219999</v>
       </c>
@@ -22948,8 +23090,9 @@
       <c r="G46" s="32">
         <v>2.821222662147</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="32">
         <v>0.93525462135199999</v>
       </c>
@@ -22968,8 +23111,9 @@
       <c r="G47" s="32">
         <v>2.8254936589519999</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="32">
         <v>1.3490006240879999</v>
       </c>
@@ -22988,8 +23132,9 @@
       <c r="G48" s="32">
         <v>2.504357829925</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H48" s="32"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="32">
         <v>1.91469172534</v>
       </c>
@@ -23008,8 +23153,9 @@
       <c r="G49" s="32">
         <v>2.6172018185889998</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H49" s="32"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="32">
         <v>1.977359599773</v>
       </c>
@@ -23028,8 +23174,9 @@
       <c r="G50" s="32">
         <v>2.6807043133790001</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="32"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="32">
         <v>1.7506292952689999</v>
       </c>
@@ -23048,8 +23195,9 @@
       <c r="G51" s="32">
         <v>2.5864940089189998</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H51" s="32"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="32">
         <v>2.0120573490060001</v>
       </c>
@@ -23068,8 +23216,9 @@
       <c r="G52" s="32">
         <v>2.8300976148469998</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H52" s="32"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="32">
         <v>1.352907219662</v>
       </c>
@@ -23088,8 +23237,9 @@
       <c r="G53" s="32">
         <v>2.7515588768420001</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H53" s="32"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="32">
         <v>1.7191290597090001</v>
       </c>
@@ -23108,8 +23258,9 @@
       <c r="G54" s="32">
         <v>2.8722329450099999</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H54" s="32"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>1.488797915261</v>
       </c>
@@ -23129,7 +23280,7 @@
         <v>2.7324787894189999</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>0.83789411432000005</v>
       </c>
@@ -23149,7 +23300,7 @@
         <v>2.9945649505519998</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>1.3962037458080001</v>
       </c>
@@ -23169,7 +23320,7 @@
         <v>2.5188166400280001</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>1.579298363865</v>
       </c>
@@ -23189,7 +23340,7 @@
         <v>3.0232450619339999</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>1.690038551609</v>
       </c>
@@ -23209,7 +23360,7 @@
         <v>3.0549890259539998</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>0.96991391764699997</v>
       </c>
@@ -23229,7 +23380,7 @@
         <v>2.7316761915769998</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>1.2345316689329999</v>
       </c>
@@ -23249,7 +23400,7 @@
         <v>2.5910552423380002</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>1.1176951398070001</v>
       </c>
@@ -23269,7 +23420,7 @@
         <v>3.123659785843</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>1.0379566818470001</v>
       </c>
@@ -23289,7 +23440,7 @@
         <v>2.739184815057</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>0.92625273208600001</v>
       </c>
@@ -23949,7 +24100,7 @@
         <v>2.9223728039960002</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>1.8290622486200001</v>
       </c>
@@ -23969,7 +24120,7 @@
         <v>2.6409784977920001</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B98">
         <v>0.87523857032399999</v>
       </c>
@@ -23989,7 +24140,7 @@
         <v>2.8395861175100001</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B99">
         <v>0.98972674342099998</v>
       </c>
@@ -24009,7 +24160,7 @@
         <v>2.7065816628010002</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B100">
         <v>1.6128448780689999</v>
       </c>
@@ -24029,7 +24180,7 @@
         <v>3.1153411507670001</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B101">
         <v>1.323200887714</v>
       </c>
@@ -24049,7 +24200,7 @@
         <v>3.003456027416</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B103">
         <v>1.4701979999999999</v>
       </c>
@@ -24068,8 +24219,11 @@
       <c r="G103">
         <v>2.799436</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H103" s="32">
+        <v>3.0836990000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B104">
         <v>0.35148990000000002</v>
       </c>
@@ -24088,8 +24242,11 @@
       <c r="G104">
         <v>0.1792936</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H104" s="32">
+        <v>0.17810860000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B105">
         <v>6.8890759999999995E-2</v>
       </c>
@@ -24108,8 +24265,11 @@
       <c r="G105">
         <v>3.5140890000000001E-2</v>
       </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H105" s="32">
+        <v>3.4908649999999999E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B106">
         <v>63</v>
       </c>
@@ -24128,8 +24288,11 @@
       <c r="G106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H106" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B107">
         <v>37</v>
       </c>
@@ -24148,29 +24311,33 @@
       <c r="G107">
         <v>99</v>
       </c>
+      <c r="H107" s="32">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O4:P4"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -24222,12 +24389,12 @@
       <c r="E2" s="32">
         <v>2.87824113329</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="32">

</xml_diff>